<commit_message>
Fix missing data in the correct place
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -606,6 +606,9 @@
       <c r="B11" s="2">
         <v>36639</v>
       </c>
+      <c r="E11">
+        <v>2.428060400516796</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
@@ -614,6 +617,9 @@
       <c r="B12" s="2">
         <v>36646</v>
       </c>
+      <c r="E12">
+        <v>3.601082715295001</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
@@ -622,6 +628,9 @@
       <c r="B13" s="2">
         <v>36653</v>
       </c>
+      <c r="E13">
+        <v>4.914803668672972</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
@@ -630,6 +639,9 @@
       <c r="B14" s="2">
         <v>36661</v>
       </c>
+      <c r="E14">
+        <v>5.974550507929128</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
@@ -638,6 +650,9 @@
       <c r="B15" s="2">
         <v>36667</v>
       </c>
+      <c r="E15">
+        <v>6.70534360788277</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
@@ -646,6 +661,9 @@
       <c r="B16" s="2">
         <v>36674</v>
       </c>
+      <c r="E16">
+        <v>7.385609112332162</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
@@ -654,6 +672,9 @@
       <c r="B17" s="2">
         <v>36681</v>
       </c>
+      <c r="E17">
+        <v>8.370199273368181</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
@@ -684,6 +705,9 @@
       <c r="B20" s="2">
         <v>36639</v>
       </c>
+      <c r="E20">
+        <v>2.285</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
@@ -692,6 +716,9 @@
       <c r="B21" s="2">
         <v>36646</v>
       </c>
+      <c r="E21">
+        <v>3.579664570230608</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
@@ -700,6 +727,9 @@
       <c r="B22" s="2">
         <v>36653</v>
       </c>
+      <c r="E22">
+        <v>4.735967184801382</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
@@ -708,6 +738,9 @@
       <c r="B23" s="2">
         <v>36661</v>
       </c>
+      <c r="E23">
+        <v>5.929332386363637</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
@@ -716,6 +749,9 @@
       <c r="B24" s="2">
         <v>36667</v>
       </c>
+      <c r="E24">
+        <v>6.604126984126984</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
@@ -724,6 +760,9 @@
       <c r="B25" s="2">
         <v>36674</v>
       </c>
+      <c r="E25">
+        <v>7.709947089947089</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
@@ -732,6 +771,9 @@
       <c r="B26" s="2">
         <v>36681</v>
       </c>
+      <c r="E26">
+        <v>8.594074074074072</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
@@ -752,7 +794,7 @@
         <v>36639</v>
       </c>
       <c r="E28">
-        <v>3.120248166580074</v>
+        <v>2.733696949168199</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -763,7 +805,7 @@
         <v>36646</v>
       </c>
       <c r="E29">
-        <v>4.280431539301513</v>
+        <v>4.246589485395448</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -774,7 +816,7 @@
         <v>36653</v>
       </c>
       <c r="E30">
-        <v>5.35892959870313</v>
+        <v>5.305275414013267</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -785,7 +827,7 @@
         <v>36661</v>
       </c>
       <c r="E31">
-        <v>5.970673860292429</v>
+        <v>5.923018800622259</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -796,7 +838,7 @@
         <v>36667</v>
       </c>
       <c r="E32">
-        <v>7.333638743631557</v>
+        <v>7.393218944221821</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -807,7 +849,7 @@
         <v>36674</v>
       </c>
       <c r="E33">
-        <v>7.938889123888614</v>
+        <v>7.756830019760492</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -818,7 +860,7 @@
         <v>36681</v>
       </c>
       <c r="E34">
-        <v>8.925237610053305</v>
+        <v>6.310178861788617</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -829,7 +871,7 @@
         <v>36688</v>
       </c>
       <c r="E35">
-        <v>9.470722853535353</v>
+        <v>6.685714285714285</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -906,7 +948,7 @@
         <v>36639</v>
       </c>
       <c r="E42">
-        <v>2.18912447257384</v>
+        <v>2.121700051647661</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -917,7 +959,7 @@
         <v>36646</v>
       </c>
       <c r="E43">
-        <v>3.429245283018868</v>
+        <v>3.386942675159236</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -928,7 +970,7 @@
         <v>36653</v>
       </c>
       <c r="E44">
-        <v>4.936791612694301</v>
+        <v>4.800179823737866</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -939,7 +981,7 @@
         <v>36661</v>
       </c>
       <c r="E45">
-        <v>6.249056186868686</v>
+        <v>6.027890833527469</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -950,7 +992,7 @@
         <v>36667</v>
       </c>
       <c r="E46">
-        <v>7.176190476190476</v>
+        <v>6.956493278341615</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -961,7 +1003,7 @@
         <v>36674</v>
       </c>
       <c r="E47">
-        <v>8.423809523809524</v>
+        <v>8.228275366779521</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -994,7 +1036,7 @@
         <v>36639</v>
       </c>
       <c r="E50">
-        <v>2.052940447297685</v>
+        <v>2.02566124813457</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1005,7 +1047,7 @@
         <v>36646</v>
       </c>
       <c r="E51">
-        <v>3.501275510204081</v>
+        <v>3.412988650693568</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1016,7 +1058,7 @@
         <v>36653</v>
       </c>
       <c r="E52">
-        <v>4.59433962264151</v>
+        <v>4.53639846743295</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1027,7 +1069,7 @@
         <v>36661</v>
       </c>
       <c r="E53">
-        <v>5.534394589244473</v>
+        <v>5.458722741433021</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1038,7 +1080,7 @@
         <v>36667</v>
       </c>
       <c r="E54">
-        <v>6.739725753999156</v>
+        <v>6.685076879747225</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1049,7 +1091,7 @@
         <v>36674</v>
       </c>
       <c r="E55">
-        <v>6.990567609181475</v>
+        <v>6.922885550245411</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1060,7 +1102,7 @@
         <v>36681</v>
       </c>
       <c r="E56">
-        <v>7.734101020675215</v>
+        <v>7.597444089456869</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1246,6 +1288,9 @@
       <c r="B73" s="2">
         <v>36546</v>
       </c>
+      <c r="E73">
+        <v>2.949916874480466</v>
+      </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
@@ -1254,6 +1299,9 @@
       <c r="B74" s="2">
         <v>36553</v>
       </c>
+      <c r="E74">
+        <v>3.827930824100736</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
@@ -1262,6 +1310,9 @@
       <c r="B75" s="2">
         <v>36558</v>
       </c>
+      <c r="E75">
+        <v>4.464450043933507</v>
+      </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
@@ -1270,6 +1321,9 @@
       <c r="B76" s="2">
         <v>36567</v>
       </c>
+      <c r="E76">
+        <v>5.203025010647008</v>
+      </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
@@ -1278,6 +1332,9 @@
       <c r="B77" s="2">
         <v>36574</v>
       </c>
+      <c r="E77">
+        <v>6.327372844651831</v>
+      </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
@@ -1286,6 +1343,9 @@
       <c r="B78" s="2">
         <v>36581</v>
       </c>
+      <c r="E78">
+        <v>6.978159283685803</v>
+      </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
@@ -1294,6 +1354,9 @@
       <c r="B79" s="2">
         <v>36588</v>
       </c>
+      <c r="E79">
+        <v>7.691452763876655</v>
+      </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
@@ -1302,6 +1365,9 @@
       <c r="B80" s="2">
         <v>36595</v>
       </c>
+      <c r="E80">
+        <v>8.496567390283554</v>
+      </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
@@ -1310,6 +1376,9 @@
       <c r="B81" s="2">
         <v>36602</v>
       </c>
+      <c r="E81">
+        <v>9.061967714048496</v>
+      </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
@@ -1318,6 +1387,9 @@
       <c r="B82" s="2">
         <v>36610</v>
       </c>
+      <c r="E82">
+        <v>10.17996756690134</v>
+      </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
@@ -1326,6 +1398,9 @@
       <c r="B83" s="2">
         <v>36616</v>
       </c>
+      <c r="E83">
+        <v>10.63377115675189</v>
+      </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
@@ -1335,7 +1410,7 @@
         <v>36630</v>
       </c>
       <c r="E84">
-        <v>12</v>
+        <v>11.8807570434624</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1367,6 +1442,9 @@
       <c r="B87" s="2">
         <v>36546</v>
       </c>
+      <c r="E87">
+        <v>2.894669277264863</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
@@ -1375,6 +1453,9 @@
       <c r="B88" s="2">
         <v>36553</v>
       </c>
+      <c r="E88">
+        <v>3.858043686174819</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
@@ -1383,6 +1464,9 @@
       <c r="B89" s="2">
         <v>36558</v>
       </c>
+      <c r="E89">
+        <v>4.307022483286293</v>
+      </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
@@ -1391,6 +1475,9 @@
       <c r="B90" s="2">
         <v>36567</v>
       </c>
+      <c r="E90">
+        <v>5.44758930969648</v>
+      </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
@@ -1399,6 +1486,9 @@
       <c r="B91" s="2">
         <v>36574</v>
       </c>
+      <c r="E91">
+        <v>6.505628853397302</v>
+      </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
@@ -1407,6 +1497,9 @@
       <c r="B92" s="2">
         <v>36581</v>
       </c>
+      <c r="E92">
+        <v>7.539993944227816</v>
+      </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
@@ -1415,6 +1508,9 @@
       <c r="B93" s="2">
         <v>36588</v>
       </c>
+      <c r="E93">
+        <v>8.239207487680615</v>
+      </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
@@ -1423,6 +1519,9 @@
       <c r="B94" s="2">
         <v>36595</v>
       </c>
+      <c r="E94">
+        <v>9.355048859934852</v>
+      </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
@@ -1431,6 +1530,9 @@
       <c r="B95" s="2">
         <v>36602</v>
       </c>
+      <c r="E95">
+        <v>9.542792712173821</v>
+      </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
@@ -1439,6 +1541,9 @@
       <c r="B96" s="2">
         <v>36610</v>
       </c>
+      <c r="E96">
+        <v>11.23461538461538</v>
+      </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
@@ -1447,6 +1552,9 @@
       <c r="B97" s="2">
         <v>36616</v>
       </c>
+      <c r="E97">
+        <v>11.02202455524931</v>
+      </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
@@ -1455,6 +1563,9 @@
       <c r="B98" s="2">
         <v>36630</v>
       </c>
+      <c r="E98">
+        <v>12.353125</v>
+      </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
@@ -1486,7 +1597,7 @@
         <v>36546</v>
       </c>
       <c r="E101">
-        <v>3.064375519026693</v>
+        <v>3.077334005038731</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -1497,7 +1608,7 @@
         <v>36553</v>
       </c>
       <c r="E102">
-        <v>4.126303013883644</v>
+        <v>4.171586641087303</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -1508,7 +1619,7 @@
         <v>36558</v>
       </c>
       <c r="E103">
-        <v>4.859282316201672</v>
+        <v>4.941293109633294</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -1519,7 +1630,7 @@
         <v>36567</v>
       </c>
       <c r="E104">
-        <v>5.636901512027431</v>
+        <v>5.662674900346253</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -1530,7 +1641,7 @@
         <v>36574</v>
       </c>
       <c r="E105">
-        <v>6.894152987959807</v>
+        <v>6.955371699194276</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -1541,7 +1652,7 @@
         <v>36581</v>
       </c>
       <c r="E106">
-        <v>7.539066891512086</v>
+        <v>7.621315192743762</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -1552,7 +1663,7 @@
         <v>36588</v>
       </c>
       <c r="E107">
-        <v>8.636567773124037</v>
+        <v>8.555380972488388</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -1563,7 +1674,7 @@
         <v>36595</v>
       </c>
       <c r="E108">
-        <v>9.180154667853566</v>
+        <v>9.246606282868557</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -1574,7 +1685,7 @@
         <v>36602</v>
       </c>
       <c r="E109">
-        <v>10.75585572116479</v>
+        <v>9.569593147751606</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -1584,9 +1695,6 @@
       <c r="B110" s="2">
         <v>36610</v>
       </c>
-      <c r="E110">
-        <v>11.48925659221426</v>
-      </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
@@ -1595,9 +1703,6 @@
       <c r="B111" s="2">
         <v>36616</v>
       </c>
-      <c r="E111">
-        <v>12.21963457047641</v>
-      </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
@@ -1607,7 +1712,7 @@
         <v>36630</v>
       </c>
       <c r="E112">
-        <v>13.60035169019963</v>
+        <v>13.75519480519481</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1618,7 +1723,7 @@
         <v>36638</v>
       </c>
       <c r="E113">
-        <v>13.41413611575108</v>
+        <v>14.05584415584416</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1629,7 +1734,7 @@
         <v>36674</v>
       </c>
       <c r="E114">
-        <v>15.89130434782609</v>
+        <v>15.97777777777778</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1684,7 +1789,7 @@
         <v>36546</v>
       </c>
       <c r="E119">
-        <v>3.58272414477179</v>
+        <v>3.580675740907558</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -1695,7 +1800,7 @@
         <v>36553</v>
       </c>
       <c r="E120">
-        <v>3.63905043229178</v>
+        <v>3.649148345781931</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -1706,7 +1811,7 @@
         <v>36558</v>
       </c>
       <c r="E121">
-        <v>4.874789756085082</v>
+        <v>4.834859223075668</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -1717,7 +1822,7 @@
         <v>36567</v>
       </c>
       <c r="E122">
-        <v>6.830815018315017</v>
+        <v>6.568385122964684</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -1728,7 +1833,7 @@
         <v>36574</v>
       </c>
       <c r="E123">
-        <v>8.518928004677191</v>
+        <v>8.289985371420514</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -1827,7 +1932,7 @@
         <v>36546</v>
       </c>
       <c r="E132">
-        <v>2.85531113000544</v>
+        <v>2.79945611300716</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -1838,7 +1943,7 @@
         <v>36553</v>
       </c>
       <c r="E133">
-        <v>4.008620918892745</v>
+        <v>3.881544929736314</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -1849,7 +1954,7 @@
         <v>36558</v>
       </c>
       <c r="E134">
-        <v>4.683063969502782</v>
+        <v>4.518611548492419</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -1860,7 +1965,7 @@
         <v>36567</v>
       </c>
       <c r="E135">
-        <v>5.289699321621002</v>
+        <v>5.183130897343855</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -1871,7 +1976,7 @@
         <v>36574</v>
       </c>
       <c r="E136">
-        <v>6.461893579972173</v>
+        <v>6.315291904060707</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -1882,7 +1987,7 @@
         <v>36581</v>
       </c>
       <c r="E137">
-        <v>6.940492443564277</v>
+        <v>6.78329595459256</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -1893,7 +1998,7 @@
         <v>36588</v>
       </c>
       <c r="E138">
-        <v>7.644492906854274</v>
+        <v>7.493957516018458</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -1904,7 +2009,7 @@
         <v>36595</v>
       </c>
       <c r="E139">
-        <v>8.486113788677581</v>
+        <v>8.34476246133107</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -1915,7 +2020,7 @@
         <v>36602</v>
       </c>
       <c r="E140">
-        <v>9.0155232076504</v>
+        <v>8.905697177312417</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -1926,7 +2031,7 @@
         <v>36610</v>
       </c>
       <c r="E141">
-        <v>10.37313875182323</v>
+        <v>10.34781949934124</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -1937,7 +2042,7 @@
         <v>36616</v>
       </c>
       <c r="E142">
-        <v>10.19104676783664</v>
+        <v>10.11325428194993</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2057,6 +2162,9 @@
       <c r="B153" s="2">
         <v>36641</v>
       </c>
+      <c r="E153">
+        <v>2.77875</v>
+      </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
@@ -2065,6 +2173,9 @@
       <c r="B154" s="2">
         <v>36648</v>
       </c>
+      <c r="E154">
+        <v>4.354672549019607</v>
+      </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="1" t="s">
@@ -2073,6 +2184,9 @@
       <c r="B155" s="2">
         <v>36653</v>
       </c>
+      <c r="E155">
+        <v>4.602333333333334</v>
+      </c>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="1" t="s">
@@ -2092,6 +2206,9 @@
       <c r="B157" s="2">
         <v>36641</v>
       </c>
+      <c r="E157">
+        <v>3.513480918489432</v>
+      </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="1" t="s">
@@ -2100,6 +2217,9 @@
       <c r="B158" s="2">
         <v>36648</v>
       </c>
+      <c r="E158">
+        <v>4.86938983845437</v>
+      </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="1" t="s">
@@ -2108,6 +2228,9 @@
       <c r="B159" s="2">
         <v>36653</v>
       </c>
+      <c r="E159">
+        <v>5.238481221538957</v>
+      </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="1" t="s">
@@ -2116,6 +2239,9 @@
       <c r="B160" s="2">
         <v>36659</v>
       </c>
+      <c r="E160">
+        <v>5.913443830570903</v>
+      </c>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="1" t="s">
@@ -2147,7 +2273,7 @@
         <v>36641</v>
       </c>
       <c r="E163">
-        <v>3.323946706887883</v>
+        <v>2.909907446501934</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -2158,7 +2284,7 @@
         <v>36648</v>
       </c>
       <c r="E164">
-        <v>4.402277807138626</v>
+        <v>4.503084953055913</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -2169,7 +2295,7 @@
         <v>36653</v>
       </c>
       <c r="E165">
-        <v>5.256666195998101</v>
+        <v>5.456542407603402</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -2180,7 +2306,7 @@
         <v>36659</v>
       </c>
       <c r="E166">
-        <v>6.052695606280512</v>
+        <v>6.277260356720665</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -2191,7 +2317,7 @@
         <v>36666</v>
       </c>
       <c r="E167">
-        <v>6.565958979494665</v>
+        <v>6.802236905136427</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -2213,7 +2339,7 @@
         <v>36641</v>
       </c>
       <c r="E169">
-        <v>2.915552044666688</v>
+        <v>2.729770442922836</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -2224,7 +2350,7 @@
         <v>36648</v>
       </c>
       <c r="E170">
-        <v>4.743010508567753</v>
+        <v>4.614949236065259</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -2235,7 +2361,7 @@
         <v>36653</v>
       </c>
       <c r="E171">
-        <v>5.832747363134104</v>
+        <v>5.693032606646981</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -2257,7 +2383,7 @@
         <v>36641</v>
       </c>
       <c r="E173">
-        <v>2.815234522477118</v>
+        <v>6.939375453885258</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -2268,7 +2394,7 @@
         <v>36648</v>
       </c>
       <c r="E174">
-        <v>4.322749860746435</v>
+        <v>3.655773420479303</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -2278,9 +2404,6 @@
       <c r="B175" s="2">
         <v>36653</v>
       </c>
-      <c r="E175">
-        <v>5.056834744225061</v>
-      </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
@@ -2289,9 +2412,6 @@
       <c r="B176" s="2">
         <v>36659</v>
       </c>
-      <c r="E176">
-        <v>5.880703114774386</v>
-      </c>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
@@ -2301,7 +2421,7 @@
         <v>36666</v>
       </c>
       <c r="E177">
-        <v>6.746069360415887</v>
+        <v>7.078125</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -2465,6 +2585,9 @@
       <c r="B192" s="2">
         <v>36533</v>
       </c>
+      <c r="E192">
+        <v>1.005691339184544</v>
+      </c>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="1" t="s">
@@ -2473,6 +2596,9 @@
       <c r="B193" s="2">
         <v>36540</v>
       </c>
+      <c r="E193">
+        <v>2.844458049379705</v>
+      </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="1" t="s">
@@ -2481,6 +2607,9 @@
       <c r="B194" s="2">
         <v>36547</v>
       </c>
+      <c r="E194">
+        <v>3.875892214906213</v>
+      </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1" t="s">
@@ -2489,6 +2618,9 @@
       <c r="B195" s="2">
         <v>36554</v>
       </c>
+      <c r="E195">
+        <v>5.194303974999472</v>
+      </c>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="1" t="s">
@@ -2497,6 +2629,9 @@
       <c r="B196" s="2">
         <v>36561</v>
       </c>
+      <c r="E196">
+        <v>6.779204073692867</v>
+      </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="1" t="s">
@@ -2516,6 +2651,9 @@
       <c r="B198" s="2">
         <v>36533</v>
       </c>
+      <c r="E198">
+        <v>1.532421694914059</v>
+      </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1" t="s">
@@ -2524,6 +2662,9 @@
       <c r="B199" s="2">
         <v>36540</v>
       </c>
+      <c r="E199">
+        <v>2.616386858944526</v>
+      </c>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1" t="s">
@@ -2532,6 +2673,9 @@
       <c r="B200" s="2">
         <v>36547</v>
       </c>
+      <c r="E200">
+        <v>4.972746375102701</v>
+      </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1" t="s">
@@ -2540,6 +2684,9 @@
       <c r="B201" s="2">
         <v>36554</v>
       </c>
+      <c r="E201">
+        <v>4.899201261515694</v>
+      </c>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="1" t="s">
@@ -2548,6 +2695,9 @@
       <c r="B202" s="2">
         <v>36561</v>
       </c>
+      <c r="E202">
+        <v>6.058783771033148</v>
+      </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="1" t="s">
@@ -2556,6 +2706,9 @@
       <c r="B203" s="2">
         <v>36568</v>
       </c>
+      <c r="E203">
+        <v>7.106542821319646</v>
+      </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
@@ -2564,6 +2717,9 @@
       <c r="B204" s="2">
         <v>36582</v>
       </c>
+      <c r="E204">
+        <v>8.479433878814683</v>
+      </c>
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="1" t="s">
@@ -2571,6 +2727,9 @@
       </c>
       <c r="B205" s="2">
         <v>36597</v>
+      </c>
+      <c r="E205">
+        <v>9.34078584891982</v>
       </c>
     </row>
     <row r="206" spans="1:5">

</xml_diff>

<commit_message>
Corrected Observed data (pivot table in source spreed sheet was not updated)
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -607,7 +607,7 @@
         <v>36639</v>
       </c>
       <c r="E11">
-        <v>2.428060400516796</v>
+        <v>2.027840351393797</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -618,7 +618,7 @@
         <v>36646</v>
       </c>
       <c r="E12">
-        <v>3.601082715295001</v>
+        <v>3.353731066541702</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -629,7 +629,7 @@
         <v>36653</v>
       </c>
       <c r="E13">
-        <v>4.914803668672972</v>
+        <v>4.719348659003832</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -640,7 +640,7 @@
         <v>36661</v>
       </c>
       <c r="E14">
-        <v>5.974550507929128</v>
+        <v>5.777999158767037</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -651,7 +651,7 @@
         <v>36667</v>
       </c>
       <c r="E15">
-        <v>6.70534360788277</v>
+        <v>6.591597796143251</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -662,7 +662,7 @@
         <v>36674</v>
       </c>
       <c r="E16">
-        <v>7.385609112332162</v>
+        <v>7.285626312069247</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -673,7 +673,7 @@
         <v>36681</v>
       </c>
       <c r="E17">
-        <v>8.370199273368181</v>
+        <v>8.164738253139552</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -706,7 +706,7 @@
         <v>36639</v>
       </c>
       <c r="E20">
-        <v>2.285</v>
+        <v>2.250978473581213</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -717,7 +717,7 @@
         <v>36646</v>
       </c>
       <c r="E21">
-        <v>3.579664570230608</v>
+        <v>3.522537971582558</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -728,7 +728,7 @@
         <v>36653</v>
       </c>
       <c r="E22">
-        <v>4.735967184801382</v>
+        <v>4.602474226804123</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -739,7 +739,7 @@
         <v>36661</v>
       </c>
       <c r="E23">
-        <v>5.929332386363637</v>
+        <v>5.662004914715236</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -750,7 +750,7 @@
         <v>36667</v>
       </c>
       <c r="E24">
-        <v>6.604126984126984</v>
+        <v>6.393929684556216</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -761,7 +761,7 @@
         <v>36674</v>
       </c>
       <c r="E25">
-        <v>7.709947089947089</v>
+        <v>7.168551106121715</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -772,7 +772,7 @@
         <v>36681</v>
       </c>
       <c r="E26">
-        <v>8.594074074074072</v>
+        <v>8.016140222803642</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -794,7 +794,7 @@
         <v>36639</v>
       </c>
       <c r="E28">
-        <v>2.733696949168199</v>
+        <v>3.120248166580074</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -805,7 +805,7 @@
         <v>36646</v>
       </c>
       <c r="E29">
-        <v>4.246589485395448</v>
+        <v>4.280431539301513</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -816,7 +816,7 @@
         <v>36653</v>
       </c>
       <c r="E30">
-        <v>5.305275414013267</v>
+        <v>5.35892959870313</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -827,7 +827,7 @@
         <v>36661</v>
       </c>
       <c r="E31">
-        <v>5.923018800622259</v>
+        <v>5.970673860292429</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -838,7 +838,7 @@
         <v>36667</v>
       </c>
       <c r="E32">
-        <v>7.393218944221821</v>
+        <v>7.333638743631557</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -849,7 +849,7 @@
         <v>36674</v>
       </c>
       <c r="E33">
-        <v>7.756830019760492</v>
+        <v>7.938889123888614</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -860,7 +860,7 @@
         <v>36681</v>
       </c>
       <c r="E34">
-        <v>6.310178861788617</v>
+        <v>8.925237610053305</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -871,7 +871,7 @@
         <v>36688</v>
       </c>
       <c r="E35">
-        <v>6.685714285714285</v>
+        <v>9.470722853535353</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -948,7 +948,7 @@
         <v>36639</v>
       </c>
       <c r="E42">
-        <v>2.121700051647661</v>
+        <v>2.18912447257384</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -959,7 +959,7 @@
         <v>36646</v>
       </c>
       <c r="E43">
-        <v>3.386942675159236</v>
+        <v>3.429245283018868</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -970,7 +970,7 @@
         <v>36653</v>
       </c>
       <c r="E44">
-        <v>4.800179823737866</v>
+        <v>4.936791612694301</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -981,7 +981,7 @@
         <v>36661</v>
       </c>
       <c r="E45">
-        <v>6.027890833527469</v>
+        <v>6.249056186868686</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -992,7 +992,7 @@
         <v>36667</v>
       </c>
       <c r="E46">
-        <v>6.956493278341615</v>
+        <v>7.176190476190476</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1003,7 +1003,7 @@
         <v>36674</v>
       </c>
       <c r="E47">
-        <v>8.228275366779521</v>
+        <v>8.423809523809524</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1036,7 +1036,7 @@
         <v>36639</v>
       </c>
       <c r="E50">
-        <v>2.02566124813457</v>
+        <v>2.052940447297685</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1047,7 +1047,7 @@
         <v>36646</v>
       </c>
       <c r="E51">
-        <v>3.412988650693568</v>
+        <v>3.501275510204081</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1058,7 +1058,7 @@
         <v>36653</v>
       </c>
       <c r="E52">
-        <v>4.53639846743295</v>
+        <v>4.59433962264151</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1069,7 +1069,7 @@
         <v>36661</v>
       </c>
       <c r="E53">
-        <v>5.458722741433021</v>
+        <v>5.534394589244473</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1080,7 +1080,7 @@
         <v>36667</v>
       </c>
       <c r="E54">
-        <v>6.685076879747225</v>
+        <v>6.739725753999156</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1091,7 +1091,7 @@
         <v>36674</v>
       </c>
       <c r="E55">
-        <v>6.922885550245411</v>
+        <v>6.990567609181475</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1102,7 +1102,7 @@
         <v>36681</v>
       </c>
       <c r="E56">
-        <v>7.597444089456869</v>
+        <v>7.734101020675215</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1289,7 +1289,7 @@
         <v>36546</v>
       </c>
       <c r="E73">
-        <v>2.949916874480466</v>
+        <v>2.781931878658861</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1300,7 +1300,7 @@
         <v>36553</v>
       </c>
       <c r="E74">
-        <v>3.827930824100736</v>
+        <v>3.690562652035528</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1311,7 +1311,7 @@
         <v>36558</v>
       </c>
       <c r="E75">
-        <v>4.464450043933507</v>
+        <v>4.36478244834977</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1322,7 +1322,7 @@
         <v>36567</v>
       </c>
       <c r="E76">
-        <v>5.203025010647008</v>
+        <v>5.082653952716075</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1333,7 +1333,7 @@
         <v>36574</v>
       </c>
       <c r="E77">
-        <v>6.327372844651831</v>
+        <v>6.238632385698204</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1344,7 +1344,7 @@
         <v>36581</v>
       </c>
       <c r="E78">
-        <v>6.978159283685803</v>
+        <v>6.801271651422589</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1355,7 +1355,7 @@
         <v>36588</v>
       </c>
       <c r="E79">
-        <v>7.691452763876655</v>
+        <v>7.622494103165831</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1366,7 +1366,7 @@
         <v>36595</v>
       </c>
       <c r="E80">
-        <v>8.496567390283554</v>
+        <v>8.399167381292468</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1377,7 +1377,7 @@
         <v>36602</v>
       </c>
       <c r="E81">
-        <v>9.061967714048496</v>
+        <v>8.986087073665527</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1388,7 +1388,7 @@
         <v>36610</v>
       </c>
       <c r="E82">
-        <v>10.17996756690134</v>
+        <v>10.08956131078224</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1399,7 +1399,7 @@
         <v>36616</v>
       </c>
       <c r="E83">
-        <v>10.63377115675189</v>
+        <v>10.53762678632404</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1410,7 +1410,7 @@
         <v>36630</v>
       </c>
       <c r="E84">
-        <v>11.8807570434624</v>
+        <v>11.88651674985288</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1443,7 +1443,7 @@
         <v>36546</v>
       </c>
       <c r="E87">
-        <v>2.894669277264863</v>
+        <v>2.860614359812277</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1454,7 +1454,7 @@
         <v>36553</v>
       </c>
       <c r="E88">
-        <v>3.858043686174819</v>
+        <v>3.926960478652095</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1465,7 +1465,7 @@
         <v>36558</v>
       </c>
       <c r="E89">
-        <v>4.307022483286293</v>
+        <v>4.303664908238337</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1476,7 +1476,7 @@
         <v>36567</v>
       </c>
       <c r="E90">
-        <v>5.44758930969648</v>
+        <v>5.3374275877576</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1487,7 +1487,7 @@
         <v>36574</v>
       </c>
       <c r="E91">
-        <v>6.505628853397302</v>
+        <v>6.229974485520966</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1498,7 +1498,7 @@
         <v>36581</v>
       </c>
       <c r="E92">
-        <v>7.539993944227816</v>
+        <v>6.918292467890037</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1509,7 +1509,7 @@
         <v>36588</v>
       </c>
       <c r="E93">
-        <v>8.239207487680615</v>
+        <v>7.557093822446562</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1520,7 +1520,7 @@
         <v>36595</v>
       </c>
       <c r="E94">
-        <v>9.355048859934852</v>
+        <v>8.434939644520483</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1531,7 +1531,7 @@
         <v>36602</v>
       </c>
       <c r="E95">
-        <v>9.542792712173821</v>
+        <v>8.785902197363226</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -1542,7 +1542,7 @@
         <v>36610</v>
       </c>
       <c r="E96">
-        <v>11.23461538461538</v>
+        <v>10.14013495013843</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -1553,7 +1553,7 @@
         <v>36616</v>
       </c>
       <c r="E97">
-        <v>11.02202455524931</v>
+        <v>10.34354844003215</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -1597,7 +1597,7 @@
         <v>36546</v>
       </c>
       <c r="E101">
-        <v>3.077334005038731</v>
+        <v>3.064375519026693</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -1608,7 +1608,7 @@
         <v>36553</v>
       </c>
       <c r="E102">
-        <v>4.171586641087303</v>
+        <v>4.126303013883644</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -1619,7 +1619,7 @@
         <v>36558</v>
       </c>
       <c r="E103">
-        <v>4.941293109633294</v>
+        <v>4.859282316201672</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -1630,7 +1630,7 @@
         <v>36567</v>
       </c>
       <c r="E104">
-        <v>5.662674900346253</v>
+        <v>5.636901512027431</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -1641,7 +1641,7 @@
         <v>36574</v>
       </c>
       <c r="E105">
-        <v>6.955371699194276</v>
+        <v>6.894152987959807</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -1652,7 +1652,7 @@
         <v>36581</v>
       </c>
       <c r="E106">
-        <v>7.621315192743762</v>
+        <v>7.539066891512086</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -1663,7 +1663,7 @@
         <v>36588</v>
       </c>
       <c r="E107">
-        <v>8.555380972488388</v>
+        <v>8.636567773124037</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -1674,7 +1674,7 @@
         <v>36595</v>
       </c>
       <c r="E108">
-        <v>9.246606282868557</v>
+        <v>9.180154667853566</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -1685,7 +1685,7 @@
         <v>36602</v>
       </c>
       <c r="E109">
-        <v>9.569593147751606</v>
+        <v>10.75585572116479</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -1695,6 +1695,9 @@
       <c r="B110" s="2">
         <v>36610</v>
       </c>
+      <c r="E110">
+        <v>11.48925659221426</v>
+      </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
@@ -1703,6 +1706,9 @@
       <c r="B111" s="2">
         <v>36616</v>
       </c>
+      <c r="E111">
+        <v>12.21963457047641</v>
+      </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
@@ -1712,7 +1718,7 @@
         <v>36630</v>
       </c>
       <c r="E112">
-        <v>13.75519480519481</v>
+        <v>13.60035169019963</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1723,7 +1729,7 @@
         <v>36638</v>
       </c>
       <c r="E113">
-        <v>14.05584415584416</v>
+        <v>13.41413611575108</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1734,7 +1740,7 @@
         <v>36674</v>
       </c>
       <c r="E114">
-        <v>15.97777777777778</v>
+        <v>15.89130434782609</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1789,7 +1795,7 @@
         <v>36546</v>
       </c>
       <c r="E119">
-        <v>3.580675740907558</v>
+        <v>3.58272414477179</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -1800,7 +1806,7 @@
         <v>36553</v>
       </c>
       <c r="E120">
-        <v>3.649148345781931</v>
+        <v>3.63905043229178</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -1811,7 +1817,7 @@
         <v>36558</v>
       </c>
       <c r="E121">
-        <v>4.834859223075668</v>
+        <v>4.874789756085082</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -1822,7 +1828,7 @@
         <v>36567</v>
       </c>
       <c r="E122">
-        <v>6.568385122964684</v>
+        <v>6.830815018315017</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -1833,7 +1839,7 @@
         <v>36574</v>
       </c>
       <c r="E123">
-        <v>8.289985371420514</v>
+        <v>8.518928004677191</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -1932,7 +1938,7 @@
         <v>36546</v>
       </c>
       <c r="E132">
-        <v>2.79945611300716</v>
+        <v>2.85531113000544</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -1943,7 +1949,7 @@
         <v>36553</v>
       </c>
       <c r="E133">
-        <v>3.881544929736314</v>
+        <v>4.008620918892745</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -1954,7 +1960,7 @@
         <v>36558</v>
       </c>
       <c r="E134">
-        <v>4.518611548492419</v>
+        <v>4.683063969502782</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -1965,7 +1971,7 @@
         <v>36567</v>
       </c>
       <c r="E135">
-        <v>5.183130897343855</v>
+        <v>5.289699321621002</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -1976,7 +1982,7 @@
         <v>36574</v>
       </c>
       <c r="E136">
-        <v>6.315291904060707</v>
+        <v>6.461893579972173</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -1987,7 +1993,7 @@
         <v>36581</v>
       </c>
       <c r="E137">
-        <v>6.78329595459256</v>
+        <v>6.940492443564277</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -1998,7 +2004,7 @@
         <v>36588</v>
       </c>
       <c r="E138">
-        <v>7.493957516018458</v>
+        <v>7.644492906854274</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -2009,7 +2015,7 @@
         <v>36595</v>
       </c>
       <c r="E139">
-        <v>8.34476246133107</v>
+        <v>8.486113788677581</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2020,7 +2026,7 @@
         <v>36602</v>
       </c>
       <c r="E140">
-        <v>8.905697177312417</v>
+        <v>9.0155232076504</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2031,7 +2037,7 @@
         <v>36610</v>
       </c>
       <c r="E141">
-        <v>10.34781949934124</v>
+        <v>10.37313875182323</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2042,7 +2048,7 @@
         <v>36616</v>
       </c>
       <c r="E142">
-        <v>10.11325428194993</v>
+        <v>10.19104676783664</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2174,7 +2180,7 @@
         <v>36648</v>
       </c>
       <c r="E154">
-        <v>4.354672549019607</v>
+        <v>4.349443790849673</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -2207,7 +2213,7 @@
         <v>36641</v>
       </c>
       <c r="E157">
-        <v>3.513480918489432</v>
+        <v>3.140414263801046</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -2218,7 +2224,7 @@
         <v>36648</v>
       </c>
       <c r="E158">
-        <v>4.86938983845437</v>
+        <v>4.728264506576705</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -2229,7 +2235,7 @@
         <v>36653</v>
       </c>
       <c r="E159">
-        <v>5.238481221538957</v>
+        <v>5.045190028431217</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -2240,7 +2246,7 @@
         <v>36659</v>
       </c>
       <c r="E160">
-        <v>5.913443830570903</v>
+        <v>6.439297583915042</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -2251,7 +2257,7 @@
         <v>36666</v>
       </c>
       <c r="E161">
-        <v>8</v>
+        <v>7.619329006326453</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -2273,7 +2279,7 @@
         <v>36641</v>
       </c>
       <c r="E163">
-        <v>2.909907446501934</v>
+        <v>3.323946706887883</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -2284,7 +2290,7 @@
         <v>36648</v>
       </c>
       <c r="E164">
-        <v>4.503084953055913</v>
+        <v>4.402277807138626</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -2295,7 +2301,7 @@
         <v>36653</v>
       </c>
       <c r="E165">
-        <v>5.456542407603402</v>
+        <v>5.256666195998101</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -2306,7 +2312,7 @@
         <v>36659</v>
       </c>
       <c r="E166">
-        <v>6.277260356720665</v>
+        <v>6.052695606280512</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -2317,7 +2323,7 @@
         <v>36666</v>
       </c>
       <c r="E167">
-        <v>6.802236905136427</v>
+        <v>6.565958979494665</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -2339,7 +2345,7 @@
         <v>36641</v>
       </c>
       <c r="E169">
-        <v>2.729770442922836</v>
+        <v>2.915552044666688</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -2350,7 +2356,7 @@
         <v>36648</v>
       </c>
       <c r="E170">
-        <v>4.614949236065259</v>
+        <v>4.743010508567753</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -2361,7 +2367,7 @@
         <v>36653</v>
       </c>
       <c r="E171">
-        <v>5.693032606646981</v>
+        <v>5.832747363134104</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -2383,7 +2389,7 @@
         <v>36641</v>
       </c>
       <c r="E173">
-        <v>6.939375453885258</v>
+        <v>2.815234522477118</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -2394,7 +2400,7 @@
         <v>36648</v>
       </c>
       <c r="E174">
-        <v>3.655773420479303</v>
+        <v>4.322749860746435</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -2404,6 +2410,9 @@
       <c r="B175" s="2">
         <v>36653</v>
       </c>
+      <c r="E175">
+        <v>5.056834744225061</v>
+      </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
@@ -2412,6 +2421,9 @@
       <c r="B176" s="2">
         <v>36659</v>
       </c>
+      <c r="E176">
+        <v>5.880703114774386</v>
+      </c>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
@@ -2421,7 +2433,7 @@
         <v>36666</v>
       </c>
       <c r="E177">
-        <v>7.078125</v>
+        <v>6.746069360415887</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -2586,7 +2598,7 @@
         <v>36533</v>
       </c>
       <c r="E192">
-        <v>1.005691339184544</v>
+        <v>1.181641482857677</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -2597,7 +2609,7 @@
         <v>36540</v>
       </c>
       <c r="E193">
-        <v>2.844458049379705</v>
+        <v>2.707680336754799</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -2608,7 +2620,7 @@
         <v>36547</v>
       </c>
       <c r="E194">
-        <v>3.875892214906213</v>
+        <v>3.928445747800587</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -2619,7 +2631,7 @@
         <v>36554</v>
       </c>
       <c r="E195">
-        <v>5.194303974999472</v>
+        <v>5.312150736911827</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -2630,7 +2642,7 @@
         <v>36561</v>
       </c>
       <c r="E196">
-        <v>6.779204073692867</v>
+        <v>7.122617526006056</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -2652,7 +2664,7 @@
         <v>36533</v>
       </c>
       <c r="E198">
-        <v>1.532421694914059</v>
+        <v>1.472210591315308</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -2663,7 +2675,7 @@
         <v>36540</v>
       </c>
       <c r="E199">
-        <v>2.616386858944526</v>
+        <v>2.737906131181342</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -2674,7 +2686,7 @@
         <v>36547</v>
       </c>
       <c r="E200">
-        <v>4.972746375102701</v>
+        <v>4.815872964956653</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -2685,7 +2697,7 @@
         <v>36554</v>
       </c>
       <c r="E201">
-        <v>4.899201261515694</v>
+        <v>4.83037663219835</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -2696,7 +2708,7 @@
         <v>36561</v>
       </c>
       <c r="E202">
-        <v>6.058783771033148</v>
+        <v>5.775715284969713</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -2707,7 +2719,7 @@
         <v>36568</v>
       </c>
       <c r="E203">
-        <v>7.106542821319646</v>
+        <v>6.674429117465286</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -2718,7 +2730,7 @@
         <v>36582</v>
       </c>
       <c r="E204">
-        <v>8.479433878814683</v>
+        <v>7.874732263606125</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -2729,7 +2741,7 @@
         <v>36597</v>
       </c>
       <c r="E205">
-        <v>9.34078584891982</v>
+        <v>8.906989015174556</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -2739,6 +2751,9 @@
       <c r="B206" s="2">
         <v>36624</v>
       </c>
+      <c r="E206">
+        <v>13.02280991735537</v>
+      </c>
     </row>
     <row r="207" spans="1:5">
       <c r="A207" s="1" t="s">
@@ -2746,6 +2761,9 @@
       </c>
       <c r="B207" s="2">
         <v>36652</v>
+      </c>
+      <c r="E207">
+        <v>13.25</v>
       </c>
     </row>
     <row r="208" spans="1:5">

</xml_diff>

<commit_message>
fixed heading in lincoln data
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Tests\Validation\Wheat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCD054B-45DC-4FAF-A674-37CB49CE0A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3630" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -29,9 +35,6 @@
   </si>
   <si>
     <t>Wheat.Structure.HaunStageFloralInitiation</t>
-  </si>
-  <si>
-    <t>Wheat.Structure.HaunStageTerminalSpikelet</t>
   </si>
   <si>
     <t>SimulationName</t>
@@ -111,15 +114,18 @@
   <si>
     <t>HarvestRipe</t>
   </si>
+  <si>
+    <t>Wheat.Phenology.HaunStageTerminalSpikelet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +189,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -229,7 +243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,9 +275,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,6 +327,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -470,16 +520,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="7" max="7" width="38.47265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -497,89 +552,89 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>36639</v>
       </c>
       <c r="E2">
-        <v>2.548333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>2.5483333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>36646</v>
       </c>
       <c r="E3">
-        <v>4.284497628288055</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>4.2844976282880554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>36653</v>
       </c>
       <c r="E4">
-        <v>5.072148206689255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>5.0721482066892554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>36661</v>
       </c>
       <c r="E5">
-        <v>6.849511931827429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>6.8495119318274291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>36667</v>
       </c>
       <c r="E6">
-        <v>7.519816024315264</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>7.5198160243152641</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>36674</v>
       </c>
       <c r="E7">
-        <v>8.819990630219396</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>8.8199906302193956</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>36681</v>
       </c>
       <c r="E8">
-        <v>9.464113878074636</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>9.4641138780746363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>36708</v>
@@ -588,9 +643,9 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>36718</v>
@@ -599,9 +654,9 @@
         <v>12.33333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>36639</v>
@@ -610,20 +665,20 @@
         <v>2.027840351393797</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <v>36646</v>
       </c>
       <c r="E12">
-        <v>3.353731066541702</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>3.3537310665417022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <v>36653</v>
@@ -632,20 +687,20 @@
         <v>4.719348659003832</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2">
         <v>36661</v>
       </c>
       <c r="E14">
-        <v>5.777999158767037</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>5.7779991587670372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
         <v>36667</v>
@@ -654,31 +709,31 @@
         <v>6.591597796143251</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2">
         <v>36674</v>
       </c>
       <c r="E16">
-        <v>7.285626312069247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>7.2856263120692466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2">
         <v>36681</v>
       </c>
       <c r="E17">
-        <v>8.164738253139552</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>8.1647382531395518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2">
         <v>36719</v>
@@ -687,9 +742,9 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2">
         <v>36722</v>
@@ -698,31 +753,31 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2">
         <v>36639</v>
       </c>
       <c r="E20">
-        <v>2.250978473581213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>2.2509784735812128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2">
         <v>36646</v>
       </c>
       <c r="E21">
-        <v>3.522537971582558</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>3.5225379715825582</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="2">
         <v>36653</v>
@@ -731,53 +786,53 @@
         <v>4.602474226804123</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2">
         <v>36661</v>
       </c>
       <c r="E23">
-        <v>5.662004914715236</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>5.6620049147152356</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2">
         <v>36667</v>
       </c>
       <c r="E24">
-        <v>6.393929684556216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>6.3939296845562161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2">
         <v>36674</v>
       </c>
       <c r="E25">
-        <v>7.168551106121715</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>7.1685511061217149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="2">
         <v>36681</v>
       </c>
       <c r="E26">
-        <v>8.016140222803642</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>8.0161402228036422</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="2">
         <v>36722</v>
@@ -786,42 +841,42 @@
         <v>12.025</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2">
         <v>36639</v>
       </c>
       <c r="E28">
-        <v>3.120248166580074</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>3.1202481665800739</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
         <v>36646</v>
       </c>
       <c r="E29">
-        <v>4.280431539301513</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>4.2804315393015129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="2">
         <v>36653</v>
       </c>
       <c r="E30">
-        <v>5.35892959870313</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>5.3589295987031296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="2">
         <v>36661</v>
@@ -830,64 +885,64 @@
         <v>5.970673860292429</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" s="2">
         <v>36667</v>
       </c>
       <c r="E32">
-        <v>7.333638743631557</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>7.3336387436315569</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B33" s="2">
         <v>36674</v>
       </c>
       <c r="E33">
-        <v>7.938889123888614</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>7.9388891238886137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" s="2">
         <v>36681</v>
       </c>
       <c r="E34">
-        <v>8.925237610053305</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>8.9252376100533048</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="2">
         <v>36688</v>
       </c>
       <c r="E35">
-        <v>9.470722853535353</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>9.4707228535353529</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="2">
         <v>36724</v>
       </c>
       <c r="E36">
-        <v>12.13333333333333</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>12.133333333333329</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="2">
         <v>36731</v>
@@ -896,20 +951,20 @@
         <v>13.66666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="2">
         <v>36738</v>
       </c>
       <c r="E38">
-        <v>13.92857142857143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>13.928571428571431</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="2">
         <v>36745</v>
@@ -918,9 +973,9 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="2">
         <v>36752</v>
@@ -929,9 +984,9 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" s="2">
         <v>36766</v>
@@ -940,31 +995,31 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="2">
         <v>36639</v>
       </c>
       <c r="E42">
-        <v>2.18912447257384</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>2.1891244725738401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="2">
         <v>36646</v>
       </c>
       <c r="E43">
-        <v>3.429245283018868</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>3.4292452830188682</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" s="2">
         <v>36653</v>
@@ -973,53 +1028,53 @@
         <v>4.936791612694301</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" s="2">
         <v>36661</v>
       </c>
       <c r="E45">
-        <v>6.249056186868686</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>6.2490561868686862</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" s="2">
         <v>36667</v>
       </c>
       <c r="E46">
-        <v>7.176190476190476</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>7.1761904761904756</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" s="2">
         <v>36674</v>
       </c>
       <c r="E47">
-        <v>8.423809523809524</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>8.4238095238095241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" s="2">
         <v>36681</v>
       </c>
       <c r="E48">
-        <v>9.333333333333334</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>9.3333333333333339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="2">
         <v>36708</v>
@@ -1028,86 +1083,86 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" s="2">
         <v>36639</v>
       </c>
       <c r="E50">
-        <v>2.052940447297685</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>2.0529404472976851</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" s="2">
         <v>36646</v>
       </c>
       <c r="E51">
-        <v>3.501275510204081</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>3.5012755102040809</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B52" s="2">
         <v>36653</v>
       </c>
       <c r="E52">
-        <v>4.59433962264151</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>4.5943396226415096</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53" s="2">
         <v>36661</v>
       </c>
       <c r="E53">
-        <v>5.534394589244473</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>5.5343945892444726</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="2">
         <v>36667</v>
       </c>
       <c r="E54">
-        <v>6.739725753999156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>6.7397257539991564</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="2">
         <v>36674</v>
       </c>
       <c r="E55">
-        <v>6.990567609181475</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>6.9905676091814746</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B56" s="2">
         <v>36681</v>
       </c>
       <c r="E56">
-        <v>7.734101020675215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>7.7341010206752152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57" s="2">
         <v>36719</v>
@@ -1116,108 +1171,108 @@
         <v>10.35</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58" s="2">
         <v>36722</v>
       </c>
       <c r="E58">
-        <v>10.1578947368421</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>10.157894736842101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B59" s="2">
         <v>36546</v>
       </c>
       <c r="E59">
-        <v>3.088689892409988</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>3.0886898924099881</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" s="2">
         <v>36553</v>
       </c>
       <c r="E60">
-        <v>4.365020053549584</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>4.3650200535495838</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B61" s="2">
         <v>36558</v>
       </c>
       <c r="E61">
-        <v>5.023279400971451</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>5.0232794009714512</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62" s="2">
         <v>36567</v>
       </c>
       <c r="E62">
-        <v>5.841277841390233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>5.8412778413902329</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B63" s="2">
         <v>36574</v>
       </c>
       <c r="E63">
-        <v>6.96598029313087</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>6.9659802931308699</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B64" s="2">
         <v>36581</v>
       </c>
       <c r="E64">
-        <v>7.990754077094318</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>7.9907540770943184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B65" s="2">
         <v>36588</v>
       </c>
       <c r="E65">
-        <v>8.633035290082811</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>8.6330352900828107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B66" s="2">
         <v>36595</v>
       </c>
       <c r="E66">
-        <v>9.859876785884474</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>9.8598767858844738</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B67" s="2">
         <v>36602</v>
@@ -1226,9 +1281,9 @@
         <v>11.22839940757212</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B68" s="2">
         <v>36610</v>
@@ -1237,9 +1292,9 @@
         <v>12.51106860614494</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B69" s="2">
         <v>36616</v>
@@ -1248,9 +1303,9 @@
         <v>12.72091443112301</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B70" s="2">
         <v>36630</v>
@@ -1259,9 +1314,9 @@
         <v>12.94225443187784</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B71" s="2">
         <v>36658</v>
@@ -1270,9 +1325,9 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B72" s="2">
         <v>36669</v>
@@ -1281,53 +1336,53 @@
         <v>16.74074074074074</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73" s="2">
         <v>36546</v>
       </c>
       <c r="E73">
-        <v>2.781931878658861</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>2.7819318786588609</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B74" s="2">
         <v>36553</v>
       </c>
       <c r="E74">
-        <v>3.690562652035528</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>3.6905626520355281</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B75" s="2">
         <v>36558</v>
       </c>
       <c r="E75">
-        <v>4.36478244834977</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>4.3647824483497697</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B76" s="2">
         <v>36567</v>
       </c>
       <c r="E76">
-        <v>5.082653952716075</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+        <v>5.0826539527160746</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B77" s="2">
         <v>36574</v>
@@ -1336,64 +1391,64 @@
         <v>6.238632385698204</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B78" s="2">
         <v>36581</v>
       </c>
       <c r="E78">
-        <v>6.801271651422589</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+        <v>6.8012716514225886</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B79" s="2">
         <v>36588</v>
       </c>
       <c r="E79">
-        <v>7.622494103165831</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+        <v>7.6224941031658311</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B80" s="2">
         <v>36595</v>
       </c>
       <c r="E80">
-        <v>8.399167381292468</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+        <v>8.3991673812924681</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B81" s="2">
         <v>36602</v>
       </c>
       <c r="E81">
-        <v>8.986087073665527</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+        <v>8.9860870736655265</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B82" s="2">
         <v>36610</v>
       </c>
       <c r="E82">
-        <v>10.08956131078224</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>10.089561310782241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B83" s="2">
         <v>36616</v>
@@ -1402,20 +1457,20 @@
         <v>10.53762678632404</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B84" s="2">
         <v>36630</v>
       </c>
       <c r="E84">
-        <v>11.88651674985288</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+        <v>11.886516749852881</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B85" s="2">
         <v>36658</v>
@@ -1424,9 +1479,9 @@
         <v>12.18333333333333</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B86" s="2">
         <v>36669</v>
@@ -1435,53 +1490,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B87" s="2">
         <v>36546</v>
       </c>
       <c r="E87">
-        <v>2.860614359812277</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+        <v>2.8606143598122769</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B88" s="2">
         <v>36553</v>
       </c>
       <c r="E88">
-        <v>3.926960478652095</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+        <v>3.9269604786520951</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" s="2">
         <v>36558</v>
       </c>
       <c r="E89">
-        <v>4.303664908238337</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+        <v>4.3036649082383374</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B90" s="2">
         <v>36567</v>
       </c>
       <c r="E90">
-        <v>5.3374275877576</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+        <v>5.3374275877575998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B91" s="2">
         <v>36574</v>
@@ -1490,9 +1545,9 @@
         <v>6.229974485520966</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B92" s="2">
         <v>36581</v>
@@ -1501,42 +1556,42 @@
         <v>6.918292467890037</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B93" s="2">
         <v>36588</v>
       </c>
       <c r="E93">
-        <v>7.557093822446562</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+        <v>7.5570938224465616</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B94" s="2">
         <v>36595</v>
       </c>
       <c r="E94">
-        <v>8.434939644520483</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+        <v>8.4349396445204832</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B95" s="2">
         <v>36602</v>
       </c>
       <c r="E95">
-        <v>8.785902197363226</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+        <v>8.7859021973632263</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B96" s="2">
         <v>36610</v>
@@ -1545,9 +1600,9 @@
         <v>10.14013495013843</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B97" s="2">
         <v>36616</v>
@@ -1556,9 +1611,9 @@
         <v>10.34354844003215</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B98" s="2">
         <v>36630</v>
@@ -1567,9 +1622,9 @@
         <v>12.353125</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B99" s="2">
         <v>36668</v>
@@ -1578,9 +1633,9 @@
         <v>13.66666666666667</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B100" s="2">
         <v>36669</v>
@@ -1589,97 +1644,97 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B101" s="2">
         <v>36546</v>
       </c>
       <c r="E101">
-        <v>3.064375519026693</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+        <v>3.0643755190266928</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B102" s="2">
         <v>36553</v>
       </c>
       <c r="E102">
-        <v>4.126303013883644</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
+        <v>4.1263030138836436</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B103" s="2">
         <v>36558</v>
       </c>
       <c r="E103">
-        <v>4.859282316201672</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+        <v>4.8592823162016723</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B104" s="2">
         <v>36567</v>
       </c>
       <c r="E104">
-        <v>5.636901512027431</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
+        <v>5.6369015120274311</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B105" s="2">
         <v>36574</v>
       </c>
       <c r="E105">
-        <v>6.894152987959807</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+        <v>6.8941529879598074</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B106" s="2">
         <v>36581</v>
       </c>
       <c r="E106">
-        <v>7.539066891512086</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+        <v>7.5390668915120864</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B107" s="2">
         <v>36588</v>
       </c>
       <c r="E107">
-        <v>8.636567773124037</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
+        <v>8.6365677731240371</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B108" s="2">
         <v>36595</v>
       </c>
       <c r="E108">
-        <v>9.180154667853566</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+        <v>9.1801546678535662</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B109" s="2">
         <v>36602</v>
@@ -1688,20 +1743,20 @@
         <v>10.75585572116479</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B110" s="2">
         <v>36610</v>
       </c>
       <c r="E110">
-        <v>11.48925659221426</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+        <v>11.489256592214261</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B111" s="2">
         <v>36616</v>
@@ -1710,31 +1765,31 @@
         <v>12.21963457047641</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B112" s="2">
         <v>36630</v>
       </c>
       <c r="E112">
-        <v>13.60035169019963</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+        <v>13.600351690199631</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="2">
         <v>36638</v>
       </c>
       <c r="E113">
-        <v>13.41413611575108</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
+        <v>13.414136115751081</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="2">
         <v>36674</v>
@@ -1743,9 +1798,9 @@
         <v>15.89130434782609</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B115" s="2">
         <v>36681</v>
@@ -1754,9 +1809,9 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B116" s="2">
         <v>36688</v>
@@ -1765,9 +1820,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B117" s="2">
         <v>36695</v>
@@ -1776,9 +1831,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B118" s="2">
         <v>36702</v>
@@ -1787,75 +1842,75 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B119" s="2">
         <v>36546</v>
       </c>
       <c r="E119">
-        <v>3.58272414477179</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
+        <v>3.5827241447717899</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B120" s="2">
         <v>36553</v>
       </c>
       <c r="E120">
-        <v>3.63905043229178</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
+        <v>3.6390504322917798</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B121" s="2">
         <v>36558</v>
       </c>
       <c r="E121">
-        <v>4.874789756085082</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
+        <v>4.8747897560850824</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B122" s="2">
         <v>36567</v>
       </c>
       <c r="E122">
-        <v>6.830815018315017</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
+        <v>6.8308150183150174</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B123" s="2">
         <v>36574</v>
       </c>
       <c r="E123">
-        <v>8.518928004677191</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
+        <v>8.5189280046771909</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B124" s="2">
         <v>36581</v>
       </c>
       <c r="E124">
-        <v>7.928571428571429</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
+        <v>7.9285714285714288</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B125" s="2">
         <v>36588</v>
@@ -1864,53 +1919,53 @@
         <v>8.125</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B126" s="2">
         <v>36595</v>
       </c>
       <c r="E126">
-        <v>8.416666666666666</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
+        <v>8.4166666666666661</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B127" s="2">
         <v>36602</v>
       </c>
       <c r="E127">
-        <v>8.666666666666666</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B128" s="2">
         <v>36610</v>
       </c>
       <c r="E128">
-        <v>8.346153846153847</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+        <v>8.3461538461538467</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B129" s="2">
         <v>36616</v>
       </c>
       <c r="E129">
-        <v>8.333333333333334</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B130" s="2">
         <v>36630</v>
@@ -1919,9 +1974,9 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B131" s="2">
         <v>36658</v>
@@ -1930,75 +1985,75 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B132" s="2">
         <v>36546</v>
       </c>
       <c r="E132">
-        <v>2.85531113000544</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+        <v>2.8553111300054401</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B133" s="2">
         <v>36553</v>
       </c>
       <c r="E133">
-        <v>4.008620918892745</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+        <v>4.0086209188927446</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B134" s="2">
         <v>36558</v>
       </c>
       <c r="E134">
-        <v>4.683063969502782</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
+        <v>4.6830639695027818</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B135" s="2">
         <v>36567</v>
       </c>
       <c r="E135">
-        <v>5.289699321621002</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
+        <v>5.2896993216210024</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B136" s="2">
         <v>36574</v>
       </c>
       <c r="E136">
-        <v>6.461893579972173</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+        <v>6.4618935799721733</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B137" s="2">
         <v>36581</v>
       </c>
       <c r="E137">
-        <v>6.940492443564277</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+        <v>6.9404924435642767</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B138" s="2">
         <v>36588</v>
@@ -2007,31 +2062,31 @@
         <v>7.644492906854274</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B139" s="2">
         <v>36595</v>
       </c>
       <c r="E139">
-        <v>8.486113788677581</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
+        <v>8.4861137886775815</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B140" s="2">
         <v>36602</v>
       </c>
       <c r="E140">
-        <v>9.0155232076504</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
+        <v>9.0155232076503999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B141" s="2">
         <v>36610</v>
@@ -2040,31 +2095,31 @@
         <v>10.37313875182323</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B142" s="2">
         <v>36616</v>
       </c>
       <c r="E142">
-        <v>10.19104676783664</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
+        <v>10.191046767836641</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B143" s="2">
         <v>36630</v>
       </c>
       <c r="E143">
-        <v>11.23607246376812</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
+        <v>11.236072463768121</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B144" s="2">
         <v>36658</v>
@@ -2073,9 +2128,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B145" s="2">
         <v>36668</v>
@@ -2084,9 +2139,9 @@
         <v>11.21875</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B146" s="2">
         <v>36669</v>
@@ -2095,20 +2150,20 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B147" s="2">
         <v>36641</v>
       </c>
       <c r="E147">
-        <v>3.242654507434944</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
+        <v>3.2426545074349442</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B148" s="2">
         <v>36648</v>
@@ -2117,9 +2172,9 @@
         <v>4.48626953737518</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B149" s="2">
         <v>36653</v>
@@ -2128,185 +2183,185 @@
         <v>5.444625222368928</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B150" s="2">
         <v>36659</v>
       </c>
       <c r="E150">
-        <v>6.69710136556002</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
+        <v>6.6971013655600196</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B151" s="2">
         <v>36666</v>
       </c>
       <c r="E151">
-        <v>8.202130640292275</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
+        <v>8.2021306402922747</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B152" s="2">
         <v>36709</v>
       </c>
       <c r="E152">
-        <v>9.157894736842104</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
+        <v>9.1578947368421044</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B153" s="2">
         <v>36641</v>
       </c>
       <c r="E153">
-        <v>2.77875</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
+        <v>2.7787500000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B154" s="2">
         <v>36648</v>
       </c>
       <c r="E154">
-        <v>4.349443790849673</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
+        <v>4.3494437908496728</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B155" s="2">
         <v>36653</v>
       </c>
       <c r="E155">
-        <v>4.602333333333334</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
+        <v>4.6023333333333341</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B156" s="2">
         <v>36709</v>
       </c>
       <c r="E156">
-        <v>7.947368421052632</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
+        <v>7.9473684210526319</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B157" s="2">
         <v>36641</v>
       </c>
       <c r="E157">
-        <v>3.140414263801046</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
+        <v>3.1404142638010462</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B158" s="2">
         <v>36648</v>
       </c>
       <c r="E158">
-        <v>4.728264506576705</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5">
+        <v>4.7282645065767053</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B159" s="2">
         <v>36653</v>
       </c>
       <c r="E159">
-        <v>5.045190028431217</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5">
+        <v>5.0451900284312172</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B160" s="2">
         <v>36659</v>
       </c>
       <c r="E160">
-        <v>6.439297583915042</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5">
+        <v>6.4392975839150424</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B161" s="2">
         <v>36666</v>
       </c>
       <c r="E161">
-        <v>7.619329006326453</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5">
+        <v>7.6193290063264527</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B162" s="2">
         <v>36709</v>
       </c>
       <c r="E162">
-        <v>8.303030303030303</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5">
+        <v>8.3030303030303028</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B163" s="2">
         <v>36641</v>
       </c>
       <c r="E163">
-        <v>3.323946706887883</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
+        <v>3.3239467068878832</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B164" s="2">
         <v>36648</v>
       </c>
       <c r="E164">
-        <v>4.402277807138626</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5">
+        <v>4.4022778071386259</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B165" s="2">
         <v>36653</v>
       </c>
       <c r="E165">
-        <v>5.256666195998101</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5">
+        <v>5.2566661959981014</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B166" s="2">
         <v>36659</v>
@@ -2315,20 +2370,20 @@
         <v>6.052695606280512</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B167" s="2">
         <v>36666</v>
       </c>
       <c r="E167">
-        <v>6.565958979494665</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5">
+        <v>6.5659589794946651</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B168" s="2">
         <v>36714</v>
@@ -2337,9 +2392,9 @@
         <v>14.27272727272727</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B169" s="2">
         <v>36641</v>
@@ -2348,53 +2403,53 @@
         <v>2.915552044666688</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B170" s="2">
         <v>36648</v>
       </c>
       <c r="E170">
-        <v>4.743010508567753</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5">
+        <v>4.7430105085677532</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B171" s="2">
         <v>36653</v>
       </c>
       <c r="E171">
-        <v>5.832747363134104</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5">
+        <v>5.8327473631341036</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B172" s="2">
         <v>36673</v>
       </c>
       <c r="E172">
-        <v>6.652173913043478</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5">
+        <v>6.6521739130434776</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B173" s="2">
         <v>36641</v>
       </c>
       <c r="E173">
-        <v>2.815234522477118</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5">
+        <v>2.8152345224771178</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B174" s="2">
         <v>36648</v>
@@ -2403,20 +2458,20 @@
         <v>4.322749860746435</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B175" s="2">
         <v>36653</v>
       </c>
       <c r="E175">
-        <v>5.056834744225061</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5">
+        <v>5.0568347442250614</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B176" s="2">
         <v>36659</v>
@@ -2425,20 +2480,20 @@
         <v>5.880703114774386</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B177" s="2">
         <v>36666</v>
       </c>
       <c r="E177">
-        <v>6.746069360415887</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
+        <v>6.7460693604158868</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B178" s="2">
         <v>36709</v>
@@ -2447,64 +2502,64 @@
         <v>7.65</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B179" s="2">
         <v>36533</v>
       </c>
       <c r="E179">
-        <v>2.068314228364868</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5">
+        <v>2.0683142283648679</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B180" s="2">
         <v>36540</v>
       </c>
       <c r="E180">
-        <v>3.738791069159557</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
+        <v>3.7387910691595572</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B181" s="2">
         <v>36547</v>
       </c>
       <c r="E181">
-        <v>4.863911726525314</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
+        <v>4.8639117265253136</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B182" s="2">
         <v>36554</v>
       </c>
       <c r="E182">
-        <v>5.459728415124984</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
+        <v>5.4597284151249843</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B183" s="2">
         <v>36561</v>
       </c>
       <c r="E183">
-        <v>6.515928154517905</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5">
+        <v>6.5159281545179049</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B184" s="2">
         <v>36568</v>
@@ -2513,9 +2568,9 @@
         <v>7.467388669728372</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B185" s="2">
         <v>36575</v>
@@ -2524,20 +2579,20 @@
         <v>8.152922315109624</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B186" s="2">
         <v>36582</v>
       </c>
       <c r="E186">
-        <v>9.147831025455895</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5">
+        <v>9.1478310254558952</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B187" s="2">
         <v>36589</v>
@@ -2546,9 +2601,9 @@
         <v>10.11607252766578</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B188" s="2">
         <v>36597</v>
@@ -2557,9 +2612,9 @@
         <v>10.44753380357443</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B189" s="2">
         <v>36634</v>
@@ -2568,9 +2623,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B190" s="2">
         <v>36639</v>
@@ -2579,9 +2634,9 @@
         <v>15.33333333333333</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B191" s="2">
         <v>36701</v>
@@ -2590,20 +2645,20 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B192" s="2">
         <v>36533</v>
       </c>
       <c r="E192">
-        <v>1.181641482857677</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5">
+        <v>1.1816414828576769</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B193" s="2">
         <v>36540</v>
@@ -2612,42 +2667,42 @@
         <v>2.707680336754799</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B194" s="2">
         <v>36547</v>
       </c>
       <c r="E194">
-        <v>3.928445747800587</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5">
+        <v>3.9284457478005872</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B195" s="2">
         <v>36554</v>
       </c>
       <c r="E195">
-        <v>5.312150736911827</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5">
+        <v>5.3121507369118266</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B196" s="2">
         <v>36561</v>
       </c>
       <c r="E196">
-        <v>7.122617526006056</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5">
+        <v>7.1226175260060556</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B197" s="2">
         <v>36582</v>
@@ -2656,20 +2711,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B198" s="2">
         <v>36533</v>
       </c>
       <c r="E198">
-        <v>1.472210591315308</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5">
+        <v>1.4722105913153081</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B199" s="2">
         <v>36540</v>
@@ -2678,9 +2733,9 @@
         <v>2.737906131181342</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B200" s="2">
         <v>36547</v>
@@ -2689,75 +2744,75 @@
         <v>4.815872964956653</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B201" s="2">
         <v>36554</v>
       </c>
       <c r="E201">
-        <v>4.83037663219835</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5">
+        <v>4.8303766321983499</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B202" s="2">
         <v>36561</v>
       </c>
       <c r="E202">
-        <v>5.775715284969713</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5">
+        <v>5.7757152849697126</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B203" s="2">
         <v>36568</v>
       </c>
       <c r="E203">
-        <v>6.674429117465286</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5">
+        <v>6.6744291174652863</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B204" s="2">
         <v>36582</v>
       </c>
       <c r="E204">
-        <v>7.874732263606125</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5">
+        <v>7.8747322636061252</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B205" s="2">
         <v>36597</v>
       </c>
       <c r="E205">
-        <v>8.906989015174556</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5">
+        <v>8.9069890151745561</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B206" s="2">
         <v>36624</v>
       </c>
       <c r="E206">
-        <v>13.02280991735537</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5">
+        <v>13.022809917355371</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B207" s="2">
         <v>36652</v>
@@ -2766,31 +2821,31 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B208" s="2">
         <v>36701</v>
       </c>
       <c r="E208">
-        <v>15.36842105263158</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5">
+        <v>15.368421052631581</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B209" s="2">
         <v>36702</v>
       </c>
       <c r="E209">
-        <v>15.85714285714286</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5">
+        <v>15.857142857142859</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B210" s="2">
         <v>36533</v>
@@ -2799,75 +2854,75 @@
         <v>0.8541131159560752</v>
       </c>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B211" s="2">
         <v>36540</v>
       </c>
       <c r="E211">
-        <v>2.698292459202806</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5">
+        <v>2.6982924592028059</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B212" s="2">
         <v>36547</v>
       </c>
       <c r="E212">
-        <v>4.062814363814502</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5">
+        <v>4.0628143638145016</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B213" s="2">
         <v>36554</v>
       </c>
       <c r="E213">
-        <v>5.410237752770962</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5">
+        <v>5.4102377527709624</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B214" s="2">
         <v>36561</v>
       </c>
       <c r="E214">
-        <v>6.026358527862616</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5">
+        <v>6.0263585278626159</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B215" s="2">
         <v>36568</v>
       </c>
       <c r="E215">
-        <v>6.857307522029155</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5">
+        <v>6.8573075220291546</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B216" s="2">
         <v>36582</v>
       </c>
       <c r="E216">
-        <v>8.640230492659885</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5">
+        <v>8.6402304926598852</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B217" s="2">
         <v>36597</v>
@@ -2876,9 +2931,9 @@
         <v>9.765006244478025</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B218" s="2">
         <v>36624</v>
@@ -2887,9 +2942,9 @@
         <v>13.20176767676768</v>
       </c>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B219" s="2">
         <v>36701</v>
@@ -2898,9 +2953,9 @@
         <v>15.52631578947368</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B220" s="2">
         <v>36707</v>
@@ -2909,31 +2964,31 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B221" s="2">
         <v>36533</v>
       </c>
       <c r="E221">
-        <v>1.49673870487824</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5">
+        <v>1.4967387048782399</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B222" s="2">
         <v>36540</v>
       </c>
       <c r="E222">
-        <v>2.586905684754522</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5">
+        <v>2.5869056847545222</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B223" s="2">
         <v>36547</v>
@@ -2942,42 +2997,42 @@
         <v>6.314511986301369</v>
       </c>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B224" s="2">
         <v>36554</v>
       </c>
       <c r="E224">
-        <v>7.102433223413776</v>
-      </c>
-    </row>
-    <row r="225" spans="1:7">
+        <v>7.1024332234137759</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B225" s="2">
         <v>36561</v>
       </c>
       <c r="E225">
-        <v>6.933333333333334</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7">
+        <v>6.9333333333333336</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B226" s="2">
         <v>36533</v>
       </c>
       <c r="E226">
-        <v>1.138451086956522</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7">
+        <v>1.1384510869565221</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B227" s="2">
         <v>36540</v>
@@ -2986,86 +3041,86 @@
         <v>2.803957718780727</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B228" s="2">
         <v>36547</v>
       </c>
       <c r="E228">
-        <v>4.5343486470189</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7">
+        <v>4.5343486470189003</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B229" s="2">
         <v>36554</v>
       </c>
       <c r="E229">
-        <v>4.823600206891333</v>
-      </c>
-    </row>
-    <row r="230" spans="1:7">
+        <v>4.8236002068913333</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B230" s="2">
         <v>36561</v>
       </c>
       <c r="E230">
-        <v>5.699357270852212</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7">
+        <v>5.6993572708522118</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B231" s="2">
         <v>36568</v>
       </c>
       <c r="E231">
-        <v>6.356375870842627</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7">
+        <v>6.3563758708426272</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B232" s="2">
         <v>36575</v>
       </c>
       <c r="E232">
-        <v>7.058105413905426</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7">
+        <v>7.0581054139054258</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B233" s="2">
         <v>36582</v>
       </c>
       <c r="E233">
-        <v>7.92618494035495</v>
-      </c>
-    </row>
-    <row r="234" spans="1:7">
+        <v>7.9261849403549496</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B234" s="2">
         <v>36597</v>
       </c>
       <c r="E234">
-        <v>8.654877351404474</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7">
+        <v>8.6548773514044743</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B235" s="2">
         <v>36634</v>
@@ -3074,9 +3129,9 @@
         <v>11.33333333333333</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B236" s="2">
         <v>36638</v>
@@ -3085,9 +3140,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B237" s="2">
         <v>36639</v>
@@ -3096,46 +3151,46 @@
         <v>11.18181818181818</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C238" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D238">
-        <v>9.136363636363637</v>
+        <v>9.1363636363636367</v>
       </c>
       <c r="F238">
-        <v>3.705785123966942</v>
+        <v>3.7057851239669422</v>
       </c>
       <c r="G238">
-        <v>5.705785123966942</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7">
+        <v>5.7057851239669422</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C239" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D239">
         <v>15.19047619047619</v>
       </c>
       <c r="F239">
-        <v>9.209523809523809</v>
+        <v>9.2095238095238088</v>
       </c>
       <c r="G239">
-        <v>11.20952380952381</v>
-      </c>
-    </row>
-    <row r="240" spans="1:7">
+        <v>11.209523809523811</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C240" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D240">
         <v>14.27272727272727</v>
@@ -3144,364 +3199,364 @@
         <v>8.375206611570249</v>
       </c>
       <c r="G240">
-        <v>10.37520661157025</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7">
+        <v>10.375206611570251</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C241" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D241">
         <v>15.625</v>
       </c>
       <c r="F241">
-        <v>9.604545454545454</v>
+        <v>9.6045454545454536</v>
       </c>
       <c r="G241">
         <v>11.60454545454545</v>
       </c>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C242" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D242">
-        <v>6.652173913043478</v>
+        <v>6.6521739130434776</v>
       </c>
       <c r="F242">
-        <v>2.229249011857707</v>
+        <v>2.2292490118577071</v>
       </c>
       <c r="G242">
-        <v>4.229249011857707</v>
-      </c>
-    </row>
-    <row r="243" spans="1:7">
+        <v>4.2292490118577071</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C243" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D243">
         <v>6.935483870967742</v>
       </c>
       <c r="F243">
-        <v>2.486803519061583</v>
+        <v>2.4868035190615831</v>
       </c>
       <c r="G243">
-        <v>4.486803519061583</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7">
+        <v>4.4868035190615831</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C244" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D244">
-        <v>7.545454545454546</v>
+        <v>7.5454545454545459</v>
       </c>
       <c r="F244">
         <v>3.041322314049586</v>
       </c>
       <c r="G244">
-        <v>5.041322314049586</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7">
+        <v>5.0413223140495864</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C245" t="s">
         <v>30</v>
-      </c>
-      <c r="C245" t="s">
-        <v>31</v>
       </c>
       <c r="D245">
         <v>10.71428571428571</v>
       </c>
       <c r="F245">
-        <v>5.92207792207792</v>
+        <v>5.9220779220779196</v>
       </c>
       <c r="G245">
-        <v>7.92207792207792</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7">
+        <v>7.9220779220779196</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C246" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D246">
-        <v>8.277777777777779</v>
+        <v>8.2777777777777786</v>
       </c>
       <c r="F246">
-        <v>2.925252525252526</v>
+        <v>2.9252525252525259</v>
       </c>
       <c r="G246">
-        <v>4.925252525252526</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7">
+        <v>4.9252525252525263</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C247" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D247">
         <v>15.5</v>
       </c>
       <c r="F247">
-        <v>9.49090909090909</v>
+        <v>9.4909090909090903</v>
       </c>
       <c r="G247">
         <v>11.49090909090909</v>
       </c>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C248" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D248">
-        <v>7.947368421052632</v>
+        <v>7.9473684210526319</v>
       </c>
       <c r="F248">
-        <v>2.62488038277512</v>
+        <v>2.6248803827751201</v>
       </c>
       <c r="G248">
-        <v>4.62488038277512</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7">
+        <v>4.6248803827751201</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C249" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D249">
         <v>8</v>
       </c>
       <c r="F249">
-        <v>2.672727272727273</v>
+        <v>2.6727272727272728</v>
       </c>
       <c r="G249">
-        <v>4.672727272727273</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7">
+        <v>4.6727272727272728</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C250" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D250">
         <v>11.34285714285714</v>
       </c>
       <c r="F250">
-        <v>3.702597402597403</v>
+        <v>3.7025974025974029</v>
       </c>
       <c r="G250">
-        <v>7.711688311688312</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7">
+        <v>7.7116883116883121</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C251" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D251">
-        <v>16.35897435897436</v>
+        <v>16.358974358974361</v>
       </c>
       <c r="F251">
-        <v>8.262703962703963</v>
+        <v>8.2627039627039629</v>
       </c>
       <c r="G251">
-        <v>12.27179487179487</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7">
+        <v>12.271794871794871</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C252" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D252">
         <v>14.24444444444444</v>
       </c>
       <c r="F252">
-        <v>8.376767676767676</v>
+        <v>8.3767676767676758</v>
       </c>
       <c r="G252">
         <v>10.34949494949495</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C253" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D253">
-        <v>16.84444444444444</v>
+        <v>16.844444444444441</v>
       </c>
       <c r="F253">
-        <v>10.74040404040404</v>
+        <v>10.740404040404041</v>
       </c>
       <c r="G253">
         <v>12.71313131313131</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C254" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D254">
-        <v>9.111111111111111</v>
+        <v>9.1111111111111107</v>
       </c>
       <c r="F254">
-        <v>2.228282828282827</v>
+        <v>2.2282828282828269</v>
       </c>
       <c r="G254">
-        <v>6.464646464646464</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7">
+        <v>6.4646464646464636</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C255" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D255">
-        <v>8.355263157894736</v>
+        <v>8.3552631578947363</v>
       </c>
       <c r="F255">
-        <v>1.541148325358851</v>
+        <v>1.5411483253588509</v>
       </c>
       <c r="G255">
         <v>5.777511961722487</v>
       </c>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C256" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D256">
-        <v>10.25641025641026</v>
+        <v>10.256410256410261</v>
       </c>
       <c r="F256">
-        <v>3.042191142191143</v>
+        <v>3.0421911421911432</v>
       </c>
       <c r="G256">
-        <v>7.505827505827506</v>
-      </c>
-    </row>
-    <row r="257" spans="1:7">
+        <v>7.5058275058275061</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C257" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D257">
-        <v>11.13333333333333</v>
+        <v>11.133333333333329</v>
       </c>
       <c r="F257">
-        <v>3.83939393939394</v>
+        <v>3.8393939393939398</v>
       </c>
       <c r="G257">
-        <v>8.303030303030303</v>
-      </c>
-    </row>
-    <row r="258" spans="1:7">
+        <v>8.3030303030303028</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C258" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D258">
         <v>12.025</v>
       </c>
       <c r="F258">
-        <v>2.922727272727274</v>
+        <v>2.9227272727272742</v>
       </c>
       <c r="G258">
         <v>8.331818181818182</v>
       </c>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C259" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D259">
         <v>13.5</v>
       </c>
       <c r="F259">
-        <v>4.263636363636364</v>
+        <v>4.2636363636363637</v>
       </c>
       <c r="G259">
         <v>9.672727272727272</v>
       </c>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C260" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D260">
         <v>11.75</v>
       </c>
       <c r="F260">
-        <v>2.627272727272728</v>
+        <v>2.6272727272727279</v>
       </c>
       <c r="G260">
         <v>8.081818181818182</v>
       </c>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C261" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D261">
-        <v>12.14102564102564</v>
+        <v>12.141025641025641</v>
       </c>
       <c r="F261">
-        <v>2.982750582750582</v>
+        <v>2.9827505827505818</v>
       </c>
       <c r="G261">
-        <v>8.437296037296036</v>
+        <v>8.4372960372960364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added HaunStage to Phenology model
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCD054B-45DC-4FAF-A674-37CB49CE0A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25798977-604E-483F-BC15-8BB13C1C17F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Wheat.Structure.FinalLeafNumber</t>
-  </si>
-  <si>
-    <t>Wheat.Structure.HaunStage</t>
   </si>
   <si>
     <t>Wheat.Structure.HaunStageFloralInitiation</t>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>Wheat.Phenology.HaunStageTerminalSpikelet</t>
+  </si>
+  <si>
+    <t>Wheat.Phenology.HaunStage</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:G261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -534,7 +534,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -546,18 +546,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>36639</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>36646</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>36653</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>36661</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>36667</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>36674</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>36681</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>36708</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>36718</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2">
         <v>36639</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>36646</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2">
         <v>36653</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>36661</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2">
         <v>36667</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2">
         <v>36674</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>36681</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2">
         <v>36719</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2">
         <v>36722</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2">
         <v>36639</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2">
         <v>36646</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2">
         <v>36653</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2">
         <v>36661</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="2">
         <v>36667</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2">
         <v>36674</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="2">
         <v>36681</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2">
         <v>36722</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2">
         <v>36639</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2">
         <v>36646</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="2">
         <v>36653</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="2">
         <v>36661</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="2">
         <v>36667</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="2">
         <v>36674</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="2">
         <v>36681</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="2">
         <v>36688</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="2">
         <v>36724</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" s="2">
         <v>36731</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" s="2">
         <v>36738</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="2">
         <v>36745</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" s="2">
         <v>36752</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" s="2">
         <v>36766</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" s="2">
         <v>36639</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" s="2">
         <v>36646</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" s="2">
         <v>36653</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" s="2">
         <v>36661</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="2">
         <v>36667</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="2">
         <v>36674</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2">
         <v>36681</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="2">
         <v>36708</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="2">
         <v>36639</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" s="2">
         <v>36646</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52" s="2">
         <v>36653</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" s="2">
         <v>36661</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="2">
         <v>36667</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="2">
         <v>36674</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56" s="2">
         <v>36681</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57" s="2">
         <v>36719</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" s="2">
         <v>36722</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" s="2">
         <v>36546</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60" s="2">
         <v>36553</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B61" s="2">
         <v>36558</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B62" s="2">
         <v>36567</v>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" s="2">
         <v>36574</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B64" s="2">
         <v>36581</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B65" s="2">
         <v>36588</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B66" s="2">
         <v>36595</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B67" s="2">
         <v>36602</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68" s="2">
         <v>36610</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B69" s="2">
         <v>36616</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B70" s="2">
         <v>36630</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B71" s="2">
         <v>36658</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B72" s="2">
         <v>36669</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B73" s="2">
         <v>36546</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B74" s="2">
         <v>36553</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B75" s="2">
         <v>36558</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B76" s="2">
         <v>36567</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B77" s="2">
         <v>36574</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B78" s="2">
         <v>36581</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B79" s="2">
         <v>36588</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B80" s="2">
         <v>36595</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B81" s="2">
         <v>36602</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B82" s="2">
         <v>36610</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B83" s="2">
         <v>36616</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B84" s="2">
         <v>36630</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B85" s="2">
         <v>36658</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B86" s="2">
         <v>36669</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B87" s="2">
         <v>36546</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B88" s="2">
         <v>36553</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B89" s="2">
         <v>36558</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B90" s="2">
         <v>36567</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B91" s="2">
         <v>36574</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B92" s="2">
         <v>36581</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B93" s="2">
         <v>36588</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B94" s="2">
         <v>36595</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B95" s="2">
         <v>36602</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B96" s="2">
         <v>36610</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B97" s="2">
         <v>36616</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B98" s="2">
         <v>36630</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B99" s="2">
         <v>36668</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B100" s="2">
         <v>36669</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B101" s="2">
         <v>36546</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B102" s="2">
         <v>36553</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B103" s="2">
         <v>36558</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B104" s="2">
         <v>36567</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B105" s="2">
         <v>36574</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B106" s="2">
         <v>36581</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B107" s="2">
         <v>36588</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B108" s="2">
         <v>36595</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B109" s="2">
         <v>36602</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B110" s="2">
         <v>36610</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B111" s="2">
         <v>36616</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B112" s="2">
         <v>36630</v>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B113" s="2">
         <v>36638</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B114" s="2">
         <v>36674</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B115" s="2">
         <v>36681</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B116" s="2">
         <v>36688</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B117" s="2">
         <v>36695</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B118" s="2">
         <v>36702</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B119" s="2">
         <v>36546</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B120" s="2">
         <v>36553</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B121" s="2">
         <v>36558</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B122" s="2">
         <v>36567</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B123" s="2">
         <v>36574</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B124" s="2">
         <v>36581</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B125" s="2">
         <v>36588</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B126" s="2">
         <v>36595</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B127" s="2">
         <v>36602</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B128" s="2">
         <v>36610</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B129" s="2">
         <v>36616</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B130" s="2">
         <v>36630</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B131" s="2">
         <v>36658</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B132" s="2">
         <v>36546</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B133" s="2">
         <v>36553</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B134" s="2">
         <v>36558</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B135" s="2">
         <v>36567</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B136" s="2">
         <v>36574</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B137" s="2">
         <v>36581</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B138" s="2">
         <v>36588</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B139" s="2">
         <v>36595</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B140" s="2">
         <v>36602</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B141" s="2">
         <v>36610</v>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B142" s="2">
         <v>36616</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B143" s="2">
         <v>36630</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B144" s="2">
         <v>36658</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B145" s="2">
         <v>36668</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B146" s="2">
         <v>36669</v>
@@ -2152,7 +2152,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B147" s="2">
         <v>36641</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B148" s="2">
         <v>36648</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B149" s="2">
         <v>36653</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B150" s="2">
         <v>36659</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B151" s="2">
         <v>36666</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B152" s="2">
         <v>36709</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B153" s="2">
         <v>36641</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B154" s="2">
         <v>36648</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B155" s="2">
         <v>36653</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B156" s="2">
         <v>36709</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B157" s="2">
         <v>36641</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B158" s="2">
         <v>36648</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B159" s="2">
         <v>36653</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B160" s="2">
         <v>36659</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B161" s="2">
         <v>36666</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B162" s="2">
         <v>36709</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B163" s="2">
         <v>36641</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B164" s="2">
         <v>36648</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B165" s="2">
         <v>36653</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B166" s="2">
         <v>36659</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B167" s="2">
         <v>36666</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B168" s="2">
         <v>36714</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B169" s="2">
         <v>36641</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B170" s="2">
         <v>36648</v>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B171" s="2">
         <v>36653</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B172" s="2">
         <v>36673</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B173" s="2">
         <v>36641</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B174" s="2">
         <v>36648</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B175" s="2">
         <v>36653</v>
@@ -2471,7 +2471,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B176" s="2">
         <v>36659</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B177" s="2">
         <v>36666</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B178" s="2">
         <v>36709</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B179" s="2">
         <v>36533</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B180" s="2">
         <v>36540</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B181" s="2">
         <v>36547</v>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B182" s="2">
         <v>36554</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B183" s="2">
         <v>36561</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B184" s="2">
         <v>36568</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B185" s="2">
         <v>36575</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B186" s="2">
         <v>36582</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B187" s="2">
         <v>36589</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B188" s="2">
         <v>36597</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B189" s="2">
         <v>36634</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B190" s="2">
         <v>36639</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B191" s="2">
         <v>36701</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B192" s="2">
         <v>36533</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B193" s="2">
         <v>36540</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B194" s="2">
         <v>36547</v>
@@ -2680,7 +2680,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B195" s="2">
         <v>36554</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B196" s="2">
         <v>36561</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B197" s="2">
         <v>36582</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B198" s="2">
         <v>36533</v>
@@ -2724,7 +2724,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B199" s="2">
         <v>36540</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B200" s="2">
         <v>36547</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B201" s="2">
         <v>36554</v>
@@ -2757,7 +2757,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B202" s="2">
         <v>36561</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B203" s="2">
         <v>36568</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B204" s="2">
         <v>36582</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B205" s="2">
         <v>36597</v>
@@ -2801,7 +2801,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B206" s="2">
         <v>36624</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B207" s="2">
         <v>36652</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B208" s="2">
         <v>36701</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B209" s="2">
         <v>36702</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B210" s="2">
         <v>36533</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B211" s="2">
         <v>36540</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B212" s="2">
         <v>36547</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B213" s="2">
         <v>36554</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B214" s="2">
         <v>36561</v>
@@ -2900,7 +2900,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B215" s="2">
         <v>36568</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B216" s="2">
         <v>36582</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B217" s="2">
         <v>36597</v>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B218" s="2">
         <v>36624</v>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B219" s="2">
         <v>36701</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B220" s="2">
         <v>36707</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B221" s="2">
         <v>36533</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B222" s="2">
         <v>36540</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B223" s="2">
         <v>36547</v>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B224" s="2">
         <v>36554</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B225" s="2">
         <v>36561</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B226" s="2">
         <v>36533</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B227" s="2">
         <v>36540</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B228" s="2">
         <v>36547</v>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B229" s="2">
         <v>36554</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B230" s="2">
         <v>36561</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B231" s="2">
         <v>36568</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B232" s="2">
         <v>36575</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B233" s="2">
         <v>36582</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B234" s="2">
         <v>36597</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B235" s="2">
         <v>36634</v>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B236" s="2">
         <v>36638</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B237" s="2">
         <v>36639</v>
@@ -3153,10 +3153,10 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C238" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D238">
         <v>9.1363636363636367</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C239" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D239">
         <v>15.19047619047619</v>
@@ -3187,10 +3187,10 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C240" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D240">
         <v>14.27272727272727</v>
@@ -3204,10 +3204,10 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C241" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D241">
         <v>15.625</v>
@@ -3221,10 +3221,10 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C242" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D242">
         <v>6.6521739130434776</v>
@@ -3238,10 +3238,10 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C243" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D243">
         <v>6.935483870967742</v>
@@ -3255,10 +3255,10 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C244" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D244">
         <v>7.5454545454545459</v>
@@ -3272,10 +3272,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C245" t="s">
         <v>29</v>
-      </c>
-      <c r="C245" t="s">
-        <v>30</v>
       </c>
       <c r="D245">
         <v>10.71428571428571</v>
@@ -3289,10 +3289,10 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C246" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D246">
         <v>8.2777777777777786</v>
@@ -3306,10 +3306,10 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C247" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D247">
         <v>15.5</v>
@@ -3323,10 +3323,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C248" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D248">
         <v>7.9473684210526319</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C249" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D249">
         <v>8</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C250" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D250">
         <v>11.34285714285714</v>
@@ -3374,10 +3374,10 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C251" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D251">
         <v>16.358974358974361</v>
@@ -3391,10 +3391,10 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C252" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D252">
         <v>14.24444444444444</v>
@@ -3408,10 +3408,10 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C253" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D253">
         <v>16.844444444444441</v>
@@ -3425,10 +3425,10 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C254" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D254">
         <v>9.1111111111111107</v>
@@ -3442,10 +3442,10 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C255" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D255">
         <v>8.3552631578947363</v>
@@ -3459,10 +3459,10 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C256" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D256">
         <v>10.256410256410261</v>
@@ -3476,10 +3476,10 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C257" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D257">
         <v>11.133333333333329</v>
@@ -3493,10 +3493,10 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C258" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D258">
         <v>12.025</v>
@@ -3510,10 +3510,10 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C259" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D259">
         <v>13.5</v>
@@ -3527,10 +3527,10 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C260" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D260">
         <v>11.75</v>
@@ -3544,10 +3544,10 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C261" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D261">
         <v>12.141025641025641</v>

</xml_diff>

<commit_message>
Fix names in observed files
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Tests\Validation\Wheat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25798977-604E-483F-BC15-8BB13C1C17F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="16605" windowHeight="10530"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -26,9 +25,6 @@
   </si>
   <si>
     <t>Wheat.Phenology.CurrentStageName</t>
-  </si>
-  <si>
-    <t>Wheat.Structure.FinalLeafNumber</t>
   </si>
   <si>
     <t>Wheat.Structure.HaunStageFloralInitiation</t>
@@ -117,11 +113,14 @@
   <si>
     <t>Wheat.Phenology.HaunStage</t>
   </si>
+  <si>
+    <t>Wheat.Phenology.FinalLeafNumber</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -276,23 +275,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -328,23 +310,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -520,21 +485,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="F268" sqref="F268"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="38.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -543,21 +509,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>36639</v>
@@ -566,9 +532,9 @@
         <v>2.5483333333333329</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>36646</v>
@@ -577,9 +543,9 @@
         <v>4.2844976282880554</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>36653</v>
@@ -588,9 +554,9 @@
         <v>5.0721482066892554</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>36661</v>
@@ -599,9 +565,9 @@
         <v>6.8495119318274291</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>36667</v>
@@ -610,9 +576,9 @@
         <v>7.5198160243152641</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2">
         <v>36674</v>
@@ -621,9 +587,9 @@
         <v>8.8199906302193956</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>36681</v>
@@ -632,9 +598,9 @@
         <v>9.4641138780746363</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
         <v>36708</v>
@@ -643,9 +609,9 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
         <v>36718</v>
@@ -654,9 +620,9 @@
         <v>12.33333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>36639</v>
@@ -665,9 +631,9 @@
         <v>2.027840351393797</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>36646</v>
@@ -676,9 +642,9 @@
         <v>3.3537310665417022</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>36653</v>
@@ -687,9 +653,9 @@
         <v>4.719348659003832</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
         <v>36661</v>
@@ -698,9 +664,9 @@
         <v>5.7779991587670372</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
         <v>36667</v>
@@ -709,9 +675,9 @@
         <v>6.591597796143251</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>36674</v>
@@ -720,9 +686,9 @@
         <v>7.2856263120692466</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2">
         <v>36681</v>
@@ -731,9 +697,9 @@
         <v>8.1647382531395518</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
         <v>36719</v>
@@ -742,9 +708,9 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
         <v>36722</v>
@@ -753,9 +719,9 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
         <v>36639</v>
@@ -764,9 +730,9 @@
         <v>2.2509784735812128</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2">
         <v>36646</v>
@@ -775,9 +741,9 @@
         <v>3.5225379715825582</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2">
         <v>36653</v>
@@ -786,9 +752,9 @@
         <v>4.602474226804123</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2">
         <v>36661</v>
@@ -797,9 +763,9 @@
         <v>5.6620049147152356</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2">
         <v>36667</v>
@@ -808,9 +774,9 @@
         <v>6.3939296845562161</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="2">
         <v>36674</v>
@@ -819,9 +785,9 @@
         <v>7.1685511061217149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2">
         <v>36681</v>
@@ -830,9 +796,9 @@
         <v>8.0161402228036422</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2">
         <v>36722</v>
@@ -841,9 +807,9 @@
         <v>12.025</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="2">
         <v>36639</v>
@@ -852,9 +818,9 @@
         <v>3.1202481665800739</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2">
         <v>36646</v>
@@ -863,9 +829,9 @@
         <v>4.2804315393015129</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="2">
         <v>36653</v>
@@ -874,9 +840,9 @@
         <v>5.3589295987031296</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="2">
         <v>36661</v>
@@ -885,9 +851,9 @@
         <v>5.970673860292429</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2">
         <v>36667</v>
@@ -896,9 +862,9 @@
         <v>7.3336387436315569</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2">
         <v>36674</v>
@@ -907,9 +873,9 @@
         <v>7.9388891238886137</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="2">
         <v>36681</v>
@@ -918,9 +884,9 @@
         <v>8.9252376100533048</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" s="2">
         <v>36688</v>
@@ -929,9 +895,9 @@
         <v>9.4707228535353529</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="2">
         <v>36724</v>
@@ -940,9 +906,9 @@
         <v>12.133333333333329</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="2">
         <v>36731</v>
@@ -951,9 +917,9 @@
         <v>13.66666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="2">
         <v>36738</v>
@@ -962,9 +928,9 @@
         <v>13.928571428571431</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="2">
         <v>36745</v>
@@ -973,9 +939,9 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="2">
         <v>36752</v>
@@ -984,9 +950,9 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" s="2">
         <v>36766</v>
@@ -995,9 +961,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" s="2">
         <v>36639</v>
@@ -1006,9 +972,9 @@
         <v>2.1891244725738401</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" s="2">
         <v>36646</v>
@@ -1017,9 +983,9 @@
         <v>3.4292452830188682</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" s="2">
         <v>36653</v>
@@ -1028,9 +994,9 @@
         <v>4.936791612694301</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="2">
         <v>36661</v>
@@ -1039,9 +1005,9 @@
         <v>6.2490561868686862</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46" s="2">
         <v>36667</v>
@@ -1050,9 +1016,9 @@
         <v>7.1761904761904756</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" s="2">
         <v>36674</v>
@@ -1061,9 +1027,9 @@
         <v>8.4238095238095241</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="2">
         <v>36681</v>
@@ -1072,9 +1038,9 @@
         <v>9.3333333333333339</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" s="2">
         <v>36708</v>
@@ -1083,9 +1049,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50" s="2">
         <v>36639</v>
@@ -1094,9 +1060,9 @@
         <v>2.0529404472976851</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B51" s="2">
         <v>36646</v>
@@ -1105,9 +1071,9 @@
         <v>3.5012755102040809</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52" s="2">
         <v>36653</v>
@@ -1116,9 +1082,9 @@
         <v>4.5943396226415096</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B53" s="2">
         <v>36661</v>
@@ -1127,9 +1093,9 @@
         <v>5.5343945892444726</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B54" s="2">
         <v>36667</v>
@@ -1138,9 +1104,9 @@
         <v>6.7397257539991564</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" s="2">
         <v>36674</v>
@@ -1149,9 +1115,9 @@
         <v>6.9905676091814746</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B56" s="2">
         <v>36681</v>
@@ -1160,9 +1126,9 @@
         <v>7.7341010206752152</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57" s="2">
         <v>36719</v>
@@ -1171,9 +1137,9 @@
         <v>10.35</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B58" s="2">
         <v>36722</v>
@@ -1182,9 +1148,9 @@
         <v>10.157894736842101</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B59" s="2">
         <v>36546</v>
@@ -1193,9 +1159,9 @@
         <v>3.0886898924099881</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" s="2">
         <v>36553</v>
@@ -1204,9 +1170,9 @@
         <v>4.3650200535495838</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61" s="2">
         <v>36558</v>
@@ -1215,9 +1181,9 @@
         <v>5.0232794009714512</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B62" s="2">
         <v>36567</v>
@@ -1226,9 +1192,9 @@
         <v>5.8412778413902329</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B63" s="2">
         <v>36574</v>
@@ -1237,9 +1203,9 @@
         <v>6.9659802931308699</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B64" s="2">
         <v>36581</v>
@@ -1248,9 +1214,9 @@
         <v>7.9907540770943184</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65" s="2">
         <v>36588</v>
@@ -1259,9 +1225,9 @@
         <v>8.6330352900828107</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66" s="2">
         <v>36595</v>
@@ -1270,9 +1236,9 @@
         <v>9.8598767858844738</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67" s="2">
         <v>36602</v>
@@ -1281,9 +1247,9 @@
         <v>11.22839940757212</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B68" s="2">
         <v>36610</v>
@@ -1292,9 +1258,9 @@
         <v>12.51106860614494</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B69" s="2">
         <v>36616</v>
@@ -1303,9 +1269,9 @@
         <v>12.72091443112301</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B70" s="2">
         <v>36630</v>
@@ -1314,9 +1280,9 @@
         <v>12.94225443187784</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B71" s="2">
         <v>36658</v>
@@ -1325,9 +1291,9 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72" s="2">
         <v>36669</v>
@@ -1336,9 +1302,9 @@
         <v>16.74074074074074</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B73" s="2">
         <v>36546</v>
@@ -1347,9 +1313,9 @@
         <v>2.7819318786588609</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B74" s="2">
         <v>36553</v>
@@ -1358,9 +1324,9 @@
         <v>3.6905626520355281</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" s="2">
         <v>36558</v>
@@ -1369,9 +1335,9 @@
         <v>4.3647824483497697</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B76" s="2">
         <v>36567</v>
@@ -1380,9 +1346,9 @@
         <v>5.0826539527160746</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77" s="2">
         <v>36574</v>
@@ -1391,9 +1357,9 @@
         <v>6.238632385698204</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B78" s="2">
         <v>36581</v>
@@ -1402,9 +1368,9 @@
         <v>6.8012716514225886</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B79" s="2">
         <v>36588</v>
@@ -1413,9 +1379,9 @@
         <v>7.6224941031658311</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B80" s="2">
         <v>36595</v>
@@ -1424,9 +1390,9 @@
         <v>8.3991673812924681</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B81" s="2">
         <v>36602</v>
@@ -1435,9 +1401,9 @@
         <v>8.9860870736655265</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B82" s="2">
         <v>36610</v>
@@ -1446,9 +1412,9 @@
         <v>10.089561310782241</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B83" s="2">
         <v>36616</v>
@@ -1457,9 +1423,9 @@
         <v>10.53762678632404</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B84" s="2">
         <v>36630</v>
@@ -1468,9 +1434,9 @@
         <v>11.886516749852881</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B85" s="2">
         <v>36658</v>
@@ -1479,9 +1445,9 @@
         <v>12.18333333333333</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B86" s="2">
         <v>36669</v>
@@ -1490,9 +1456,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B87" s="2">
         <v>36546</v>
@@ -1501,9 +1467,9 @@
         <v>2.8606143598122769</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B88" s="2">
         <v>36553</v>
@@ -1512,9 +1478,9 @@
         <v>3.9269604786520951</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B89" s="2">
         <v>36558</v>
@@ -1523,9 +1489,9 @@
         <v>4.3036649082383374</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B90" s="2">
         <v>36567</v>
@@ -1534,9 +1500,9 @@
         <v>5.3374275877575998</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B91" s="2">
         <v>36574</v>
@@ -1545,9 +1511,9 @@
         <v>6.229974485520966</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B92" s="2">
         <v>36581</v>
@@ -1556,9 +1522,9 @@
         <v>6.918292467890037</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B93" s="2">
         <v>36588</v>
@@ -1567,9 +1533,9 @@
         <v>7.5570938224465616</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B94" s="2">
         <v>36595</v>
@@ -1578,9 +1544,9 @@
         <v>8.4349396445204832</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B95" s="2">
         <v>36602</v>
@@ -1589,9 +1555,9 @@
         <v>8.7859021973632263</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B96" s="2">
         <v>36610</v>
@@ -1600,9 +1566,9 @@
         <v>10.14013495013843</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B97" s="2">
         <v>36616</v>
@@ -1611,9 +1577,9 @@
         <v>10.34354844003215</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B98" s="2">
         <v>36630</v>
@@ -1622,9 +1588,9 @@
         <v>12.353125</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B99" s="2">
         <v>36668</v>
@@ -1633,9 +1599,9 @@
         <v>13.66666666666667</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B100" s="2">
         <v>36669</v>
@@ -1644,9 +1610,9 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B101" s="2">
         <v>36546</v>
@@ -1655,9 +1621,9 @@
         <v>3.0643755190266928</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B102" s="2">
         <v>36553</v>
@@ -1666,9 +1632,9 @@
         <v>4.1263030138836436</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B103" s="2">
         <v>36558</v>
@@ -1677,9 +1643,9 @@
         <v>4.8592823162016723</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B104" s="2">
         <v>36567</v>
@@ -1688,9 +1654,9 @@
         <v>5.6369015120274311</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B105" s="2">
         <v>36574</v>
@@ -1699,9 +1665,9 @@
         <v>6.8941529879598074</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B106" s="2">
         <v>36581</v>
@@ -1710,9 +1676,9 @@
         <v>7.5390668915120864</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B107" s="2">
         <v>36588</v>
@@ -1721,9 +1687,9 @@
         <v>8.6365677731240371</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B108" s="2">
         <v>36595</v>
@@ -1732,9 +1698,9 @@
         <v>9.1801546678535662</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B109" s="2">
         <v>36602</v>
@@ -1743,9 +1709,9 @@
         <v>10.75585572116479</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B110" s="2">
         <v>36610</v>
@@ -1754,9 +1720,9 @@
         <v>11.489256592214261</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B111" s="2">
         <v>36616</v>
@@ -1765,9 +1731,9 @@
         <v>12.21963457047641</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B112" s="2">
         <v>36630</v>
@@ -1776,9 +1742,9 @@
         <v>13.600351690199631</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B113" s="2">
         <v>36638</v>
@@ -1787,9 +1753,9 @@
         <v>13.414136115751081</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B114" s="2">
         <v>36674</v>
@@ -1798,9 +1764,9 @@
         <v>15.89130434782609</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B115" s="2">
         <v>36681</v>
@@ -1809,9 +1775,9 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B116" s="2">
         <v>36688</v>
@@ -1820,9 +1786,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B117" s="2">
         <v>36695</v>
@@ -1831,9 +1797,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B118" s="2">
         <v>36702</v>
@@ -1842,9 +1808,9 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B119" s="2">
         <v>36546</v>
@@ -1853,9 +1819,9 @@
         <v>3.5827241447717899</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B120" s="2">
         <v>36553</v>
@@ -1864,9 +1830,9 @@
         <v>3.6390504322917798</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B121" s="2">
         <v>36558</v>
@@ -1875,9 +1841,9 @@
         <v>4.8747897560850824</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B122" s="2">
         <v>36567</v>
@@ -1886,9 +1852,9 @@
         <v>6.8308150183150174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B123" s="2">
         <v>36574</v>
@@ -1897,9 +1863,9 @@
         <v>8.5189280046771909</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B124" s="2">
         <v>36581</v>
@@ -1908,9 +1874,9 @@
         <v>7.9285714285714288</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B125" s="2">
         <v>36588</v>
@@ -1919,9 +1885,9 @@
         <v>8.125</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B126" s="2">
         <v>36595</v>
@@ -1930,9 +1896,9 @@
         <v>8.4166666666666661</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B127" s="2">
         <v>36602</v>
@@ -1941,9 +1907,9 @@
         <v>8.6666666666666661</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B128" s="2">
         <v>36610</v>
@@ -1952,9 +1918,9 @@
         <v>8.3461538461538467</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B129" s="2">
         <v>36616</v>
@@ -1963,9 +1929,9 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B130" s="2">
         <v>36630</v>
@@ -1974,9 +1940,9 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B131" s="2">
         <v>36658</v>
@@ -1985,9 +1951,9 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B132" s="2">
         <v>36546</v>
@@ -1996,9 +1962,9 @@
         <v>2.8553111300054401</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B133" s="2">
         <v>36553</v>
@@ -2007,9 +1973,9 @@
         <v>4.0086209188927446</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B134" s="2">
         <v>36558</v>
@@ -2018,9 +1984,9 @@
         <v>4.6830639695027818</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B135" s="2">
         <v>36567</v>
@@ -2029,9 +1995,9 @@
         <v>5.2896993216210024</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B136" s="2">
         <v>36574</v>
@@ -2040,9 +2006,9 @@
         <v>6.4618935799721733</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B137" s="2">
         <v>36581</v>
@@ -2051,9 +2017,9 @@
         <v>6.9404924435642767</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B138" s="2">
         <v>36588</v>
@@ -2062,9 +2028,9 @@
         <v>7.644492906854274</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B139" s="2">
         <v>36595</v>
@@ -2073,9 +2039,9 @@
         <v>8.4861137886775815</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B140" s="2">
         <v>36602</v>
@@ -2084,9 +2050,9 @@
         <v>9.0155232076503999</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B141" s="2">
         <v>36610</v>
@@ -2095,9 +2061,9 @@
         <v>10.37313875182323</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B142" s="2">
         <v>36616</v>
@@ -2106,9 +2072,9 @@
         <v>10.191046767836641</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B143" s="2">
         <v>36630</v>
@@ -2117,9 +2083,9 @@
         <v>11.236072463768121</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B144" s="2">
         <v>36658</v>
@@ -2128,9 +2094,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B145" s="2">
         <v>36668</v>
@@ -2139,9 +2105,9 @@
         <v>11.21875</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B146" s="2">
         <v>36669</v>
@@ -2150,9 +2116,9 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B147" s="2">
         <v>36641</v>
@@ -2161,9 +2127,9 @@
         <v>3.2426545074349442</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B148" s="2">
         <v>36648</v>
@@ -2172,9 +2138,9 @@
         <v>4.48626953737518</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B149" s="2">
         <v>36653</v>
@@ -2183,9 +2149,9 @@
         <v>5.444625222368928</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B150" s="2">
         <v>36659</v>
@@ -2194,9 +2160,9 @@
         <v>6.6971013655600196</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B151" s="2">
         <v>36666</v>
@@ -2205,9 +2171,9 @@
         <v>8.2021306402922747</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B152" s="2">
         <v>36709</v>
@@ -2216,9 +2182,9 @@
         <v>9.1578947368421044</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B153" s="2">
         <v>36641</v>
@@ -2227,9 +2193,9 @@
         <v>2.7787500000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B154" s="2">
         <v>36648</v>
@@ -2238,9 +2204,9 @@
         <v>4.3494437908496728</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B155" s="2">
         <v>36653</v>
@@ -2249,9 +2215,9 @@
         <v>4.6023333333333341</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B156" s="2">
         <v>36709</v>
@@ -2260,9 +2226,9 @@
         <v>7.9473684210526319</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B157" s="2">
         <v>36641</v>
@@ -2271,9 +2237,9 @@
         <v>3.1404142638010462</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B158" s="2">
         <v>36648</v>
@@ -2282,9 +2248,9 @@
         <v>4.7282645065767053</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B159" s="2">
         <v>36653</v>
@@ -2293,9 +2259,9 @@
         <v>5.0451900284312172</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B160" s="2">
         <v>36659</v>
@@ -2304,9 +2270,9 @@
         <v>6.4392975839150424</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B161" s="2">
         <v>36666</v>
@@ -2315,9 +2281,9 @@
         <v>7.6193290063264527</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B162" s="2">
         <v>36709</v>
@@ -2326,9 +2292,9 @@
         <v>8.3030303030303028</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B163" s="2">
         <v>36641</v>
@@ -2337,9 +2303,9 @@
         <v>3.3239467068878832</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B164" s="2">
         <v>36648</v>
@@ -2348,9 +2314,9 @@
         <v>4.4022778071386259</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B165" s="2">
         <v>36653</v>
@@ -2359,9 +2325,9 @@
         <v>5.2566661959981014</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B166" s="2">
         <v>36659</v>
@@ -2370,9 +2336,9 @@
         <v>6.052695606280512</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B167" s="2">
         <v>36666</v>
@@ -2381,9 +2347,9 @@
         <v>6.5659589794946651</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B168" s="2">
         <v>36714</v>
@@ -2392,9 +2358,9 @@
         <v>14.27272727272727</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B169" s="2">
         <v>36641</v>
@@ -2403,9 +2369,9 @@
         <v>2.915552044666688</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B170" s="2">
         <v>36648</v>
@@ -2414,9 +2380,9 @@
         <v>4.7430105085677532</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B171" s="2">
         <v>36653</v>
@@ -2425,9 +2391,9 @@
         <v>5.8327473631341036</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B172" s="2">
         <v>36673</v>
@@ -2436,9 +2402,9 @@
         <v>6.6521739130434776</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B173" s="2">
         <v>36641</v>
@@ -2447,9 +2413,9 @@
         <v>2.8152345224771178</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B174" s="2">
         <v>36648</v>
@@ -2458,9 +2424,9 @@
         <v>4.322749860746435</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B175" s="2">
         <v>36653</v>
@@ -2469,9 +2435,9 @@
         <v>5.0568347442250614</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B176" s="2">
         <v>36659</v>
@@ -2480,9 +2446,9 @@
         <v>5.880703114774386</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B177" s="2">
         <v>36666</v>
@@ -2491,9 +2457,9 @@
         <v>6.7460693604158868</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B178" s="2">
         <v>36709</v>
@@ -2502,9 +2468,9 @@
         <v>7.65</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B179" s="2">
         <v>36533</v>
@@ -2513,9 +2479,9 @@
         <v>2.0683142283648679</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B180" s="2">
         <v>36540</v>
@@ -2524,9 +2490,9 @@
         <v>3.7387910691595572</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B181" s="2">
         <v>36547</v>
@@ -2535,9 +2501,9 @@
         <v>4.8639117265253136</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B182" s="2">
         <v>36554</v>
@@ -2546,9 +2512,9 @@
         <v>5.4597284151249843</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B183" s="2">
         <v>36561</v>
@@ -2557,9 +2523,9 @@
         <v>6.5159281545179049</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B184" s="2">
         <v>36568</v>
@@ -2568,9 +2534,9 @@
         <v>7.467388669728372</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B185" s="2">
         <v>36575</v>
@@ -2579,9 +2545,9 @@
         <v>8.152922315109624</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B186" s="2">
         <v>36582</v>
@@ -2590,9 +2556,9 @@
         <v>9.1478310254558952</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B187" s="2">
         <v>36589</v>
@@ -2601,9 +2567,9 @@
         <v>10.11607252766578</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B188" s="2">
         <v>36597</v>
@@ -2612,9 +2578,9 @@
         <v>10.44753380357443</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B189" s="2">
         <v>36634</v>
@@ -2623,9 +2589,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B190" s="2">
         <v>36639</v>
@@ -2634,9 +2600,9 @@
         <v>15.33333333333333</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B191" s="2">
         <v>36701</v>
@@ -2645,9 +2611,9 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B192" s="2">
         <v>36533</v>
@@ -2656,9 +2622,9 @@
         <v>1.1816414828576769</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B193" s="2">
         <v>36540</v>
@@ -2667,9 +2633,9 @@
         <v>2.707680336754799</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B194" s="2">
         <v>36547</v>
@@ -2678,9 +2644,9 @@
         <v>3.9284457478005872</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B195" s="2">
         <v>36554</v>
@@ -2689,9 +2655,9 @@
         <v>5.3121507369118266</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B196" s="2">
         <v>36561</v>
@@ -2700,9 +2666,9 @@
         <v>7.1226175260060556</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B197" s="2">
         <v>36582</v>
@@ -2711,9 +2677,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B198" s="2">
         <v>36533</v>
@@ -2722,9 +2688,9 @@
         <v>1.4722105913153081</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B199" s="2">
         <v>36540</v>
@@ -2733,9 +2699,9 @@
         <v>2.737906131181342</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B200" s="2">
         <v>36547</v>
@@ -2744,9 +2710,9 @@
         <v>4.815872964956653</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B201" s="2">
         <v>36554</v>
@@ -2755,9 +2721,9 @@
         <v>4.8303766321983499</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B202" s="2">
         <v>36561</v>
@@ -2766,9 +2732,9 @@
         <v>5.7757152849697126</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B203" s="2">
         <v>36568</v>
@@ -2777,9 +2743,9 @@
         <v>6.6744291174652863</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B204" s="2">
         <v>36582</v>
@@ -2788,9 +2754,9 @@
         <v>7.8747322636061252</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B205" s="2">
         <v>36597</v>
@@ -2799,9 +2765,9 @@
         <v>8.9069890151745561</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B206" s="2">
         <v>36624</v>
@@ -2810,9 +2776,9 @@
         <v>13.022809917355371</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B207" s="2">
         <v>36652</v>
@@ -2821,9 +2787,9 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B208" s="2">
         <v>36701</v>
@@ -2832,9 +2798,9 @@
         <v>15.368421052631581</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B209" s="2">
         <v>36702</v>
@@ -2843,9 +2809,9 @@
         <v>15.857142857142859</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B210" s="2">
         <v>36533</v>
@@ -2854,9 +2820,9 @@
         <v>0.8541131159560752</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B211" s="2">
         <v>36540</v>
@@ -2865,9 +2831,9 @@
         <v>2.6982924592028059</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B212" s="2">
         <v>36547</v>
@@ -2876,9 +2842,9 @@
         <v>4.0628143638145016</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B213" s="2">
         <v>36554</v>
@@ -2887,9 +2853,9 @@
         <v>5.4102377527709624</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B214" s="2">
         <v>36561</v>
@@ -2898,9 +2864,9 @@
         <v>6.0263585278626159</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B215" s="2">
         <v>36568</v>
@@ -2909,9 +2875,9 @@
         <v>6.8573075220291546</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B216" s="2">
         <v>36582</v>
@@ -2920,9 +2886,9 @@
         <v>8.6402304926598852</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B217" s="2">
         <v>36597</v>
@@ -2931,9 +2897,9 @@
         <v>9.765006244478025</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B218" s="2">
         <v>36624</v>
@@ -2942,9 +2908,9 @@
         <v>13.20176767676768</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B219" s="2">
         <v>36701</v>
@@ -2953,9 +2919,9 @@
         <v>15.52631578947368</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B220" s="2">
         <v>36707</v>
@@ -2964,9 +2930,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B221" s="2">
         <v>36533</v>
@@ -2975,9 +2941,9 @@
         <v>1.4967387048782399</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B222" s="2">
         <v>36540</v>
@@ -2986,9 +2952,9 @@
         <v>2.5869056847545222</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B223" s="2">
         <v>36547</v>
@@ -2997,9 +2963,9 @@
         <v>6.314511986301369</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B224" s="2">
         <v>36554</v>
@@ -3008,9 +2974,9 @@
         <v>7.1024332234137759</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B225" s="2">
         <v>36561</v>
@@ -3019,9 +2985,9 @@
         <v>6.9333333333333336</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B226" s="2">
         <v>36533</v>
@@ -3030,9 +2996,9 @@
         <v>1.1384510869565221</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B227" s="2">
         <v>36540</v>
@@ -3041,9 +3007,9 @@
         <v>2.803957718780727</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B228" s="2">
         <v>36547</v>
@@ -3052,9 +3018,9 @@
         <v>4.5343486470189003</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B229" s="2">
         <v>36554</v>
@@ -3063,9 +3029,9 @@
         <v>4.8236002068913333</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B230" s="2">
         <v>36561</v>
@@ -3074,9 +3040,9 @@
         <v>5.6993572708522118</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B231" s="2">
         <v>36568</v>
@@ -3085,9 +3051,9 @@
         <v>6.3563758708426272</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B232" s="2">
         <v>36575</v>
@@ -3096,9 +3062,9 @@
         <v>7.0581054139054258</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B233" s="2">
         <v>36582</v>
@@ -3107,9 +3073,9 @@
         <v>7.9261849403549496</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B234" s="2">
         <v>36597</v>
@@ -3118,9 +3084,9 @@
         <v>8.6548773514044743</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B235" s="2">
         <v>36634</v>
@@ -3129,9 +3095,9 @@
         <v>11.33333333333333</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B236" s="2">
         <v>36638</v>
@@ -3140,9 +3106,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B237" s="2">
         <v>36639</v>
@@ -3151,12 +3117,12 @@
         <v>11.18181818181818</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C238" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D238">
         <v>9.1363636363636367</v>
@@ -3168,12 +3134,12 @@
         <v>5.7057851239669422</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C239" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D239">
         <v>15.19047619047619</v>
@@ -3185,12 +3151,12 @@
         <v>11.209523809523811</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C240" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D240">
         <v>14.27272727272727</v>
@@ -3202,12 +3168,12 @@
         <v>10.375206611570251</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C241" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D241">
         <v>15.625</v>
@@ -3219,12 +3185,12 @@
         <v>11.60454545454545</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C242" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D242">
         <v>6.6521739130434776</v>
@@ -3236,12 +3202,12 @@
         <v>4.2292490118577071</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C243" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D243">
         <v>6.935483870967742</v>
@@ -3253,12 +3219,12 @@
         <v>4.4868035190615831</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C244" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D244">
         <v>7.5454545454545459</v>
@@ -3270,12 +3236,12 @@
         <v>5.0413223140495864</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C245" t="s">
         <v>28</v>
-      </c>
-      <c r="C245" t="s">
-        <v>29</v>
       </c>
       <c r="D245">
         <v>10.71428571428571</v>
@@ -3287,12 +3253,12 @@
         <v>7.9220779220779196</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C246" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D246">
         <v>8.2777777777777786</v>
@@ -3304,12 +3270,12 @@
         <v>4.9252525252525263</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C247" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D247">
         <v>15.5</v>
@@ -3321,12 +3287,12 @@
         <v>11.49090909090909</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C248" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D248">
         <v>7.9473684210526319</v>
@@ -3338,12 +3304,12 @@
         <v>4.6248803827751201</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C249" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D249">
         <v>8</v>
@@ -3355,12 +3321,12 @@
         <v>4.6727272727272728</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C250" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D250">
         <v>11.34285714285714</v>
@@ -3372,12 +3338,12 @@
         <v>7.7116883116883121</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C251" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D251">
         <v>16.358974358974361</v>
@@ -3389,12 +3355,12 @@
         <v>12.271794871794871</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C252" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D252">
         <v>14.24444444444444</v>
@@ -3406,12 +3372,12 @@
         <v>10.34949494949495</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C253" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D253">
         <v>16.844444444444441</v>
@@ -3423,12 +3389,12 @@
         <v>12.71313131313131</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C254" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D254">
         <v>9.1111111111111107</v>
@@ -3440,12 +3406,12 @@
         <v>6.4646464646464636</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C255" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D255">
         <v>8.3552631578947363</v>
@@ -3457,12 +3423,12 @@
         <v>5.777511961722487</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C256" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D256">
         <v>10.256410256410261</v>
@@ -3474,12 +3440,12 @@
         <v>7.5058275058275061</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C257" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D257">
         <v>11.133333333333329</v>
@@ -3491,12 +3457,12 @@
         <v>8.3030303030303028</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C258" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D258">
         <v>12.025</v>
@@ -3508,12 +3474,12 @@
         <v>8.331818181818182</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C259" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D259">
         <v>13.5</v>
@@ -3525,12 +3491,12 @@
         <v>9.672727272727272</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C260" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D260">
         <v>11.75</v>
@@ -3542,12 +3508,12 @@
         <v>8.081818181818182</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C261" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D261">
         <v>12.141025641025641</v>

</xml_diff>

<commit_message>
Model working better.  Progress with checking results and fitting
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE8FC9-537E-4DFE-BD83-973DEF0F0569}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16605" windowHeight="10530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -25,9 +26,6 @@
   </si>
   <si>
     <t>Wheat.Phenology.CurrentStageName</t>
-  </si>
-  <si>
-    <t>Wheat.Structure.HaunStageFloralInitiation</t>
   </si>
   <si>
     <t>SimulationName</t>
@@ -108,19 +106,22 @@
     <t>HarvestRipe</t>
   </si>
   <si>
-    <t>Wheat.Phenology.HaunStageTerminalSpikelet</t>
+    <t>Wheat.Leaf.HaunStage</t>
   </si>
   <si>
-    <t>Wheat.Phenology.HaunStage</t>
+    <t>Wheat.Leaf.FinalLeafNumber</t>
   </si>
   <si>
-    <t>Wheat.Phenology.FinalLeafNumber</t>
+    <t>Wheat.Phenology.CAMP.TSHS</t>
+  </si>
+  <si>
+    <t>Wheat.Phenology.CAMP.VSHS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -275,6 +276,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -310,6 +328,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -485,11 +520,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="F268" sqref="F268"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +535,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -509,21 +544,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>36639</v>
@@ -534,7 +569,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>36646</v>
@@ -545,7 +580,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>36653</v>
@@ -556,7 +591,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>36661</v>
@@ -567,7 +602,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2">
         <v>36667</v>
@@ -578,7 +613,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2">
         <v>36674</v>
@@ -589,7 +624,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
         <v>36681</v>
@@ -600,7 +635,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
         <v>36708</v>
@@ -611,7 +646,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
         <v>36718</v>
@@ -622,7 +657,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2">
         <v>36639</v>
@@ -633,7 +668,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
         <v>36646</v>
@@ -644,7 +679,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="2">
         <v>36653</v>
@@ -655,7 +690,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="2">
         <v>36661</v>
@@ -666,7 +701,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2">
         <v>36667</v>
@@ -677,7 +712,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="2">
         <v>36674</v>
@@ -688,7 +723,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2">
         <v>36681</v>
@@ -699,7 +734,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2">
         <v>36719</v>
@@ -710,7 +745,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
         <v>36722</v>
@@ -721,7 +756,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>36639</v>
@@ -732,7 +767,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>36646</v>
@@ -743,7 +778,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>36653</v>
@@ -754,7 +789,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
         <v>36661</v>
@@ -765,7 +800,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
         <v>36667</v>
@@ -776,7 +811,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
         <v>36674</v>
@@ -787,7 +822,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>36681</v>
@@ -798,7 +833,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>36722</v>
@@ -809,7 +844,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2">
         <v>36639</v>
@@ -820,7 +855,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="2">
         <v>36646</v>
@@ -831,7 +866,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2">
         <v>36653</v>
@@ -842,7 +877,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="2">
         <v>36661</v>
@@ -853,7 +888,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="2">
         <v>36667</v>
@@ -864,7 +899,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="2">
         <v>36674</v>
@@ -875,7 +910,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="2">
         <v>36681</v>
@@ -886,7 +921,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="2">
         <v>36688</v>
@@ -897,7 +932,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" s="2">
         <v>36724</v>
@@ -908,7 +943,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" s="2">
         <v>36731</v>
@@ -919,7 +954,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="2">
         <v>36738</v>
@@ -930,7 +965,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" s="2">
         <v>36745</v>
@@ -941,7 +976,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40" s="2">
         <v>36752</v>
@@ -952,7 +987,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" s="2">
         <v>36766</v>
@@ -963,7 +998,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B42" s="2">
         <v>36639</v>
@@ -974,7 +1009,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43" s="2">
         <v>36646</v>
@@ -985,7 +1020,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B44" s="2">
         <v>36653</v>
@@ -996,7 +1031,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" s="2">
         <v>36661</v>
@@ -1007,7 +1042,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" s="2">
         <v>36667</v>
@@ -1018,7 +1053,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B47" s="2">
         <v>36674</v>
@@ -1029,7 +1064,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" s="2">
         <v>36681</v>
@@ -1040,7 +1075,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" s="2">
         <v>36708</v>
@@ -1051,7 +1086,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" s="2">
         <v>36639</v>
@@ -1062,7 +1097,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" s="2">
         <v>36646</v>
@@ -1073,7 +1108,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="2">
         <v>36653</v>
@@ -1084,7 +1119,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53" s="2">
         <v>36661</v>
@@ -1095,7 +1130,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" s="2">
         <v>36667</v>
@@ -1106,7 +1141,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55" s="2">
         <v>36674</v>
@@ -1117,7 +1152,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" s="2">
         <v>36681</v>
@@ -1128,7 +1163,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" s="2">
         <v>36719</v>
@@ -1139,7 +1174,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" s="2">
         <v>36722</v>
@@ -1150,7 +1185,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B59" s="2">
         <v>36546</v>
@@ -1161,7 +1196,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B60" s="2">
         <v>36553</v>
@@ -1172,7 +1207,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B61" s="2">
         <v>36558</v>
@@ -1183,7 +1218,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62" s="2">
         <v>36567</v>
@@ -1194,7 +1229,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B63" s="2">
         <v>36574</v>
@@ -1205,7 +1240,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B64" s="2">
         <v>36581</v>
@@ -1216,7 +1251,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B65" s="2">
         <v>36588</v>
@@ -1227,7 +1262,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66" s="2">
         <v>36595</v>
@@ -1238,7 +1273,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B67" s="2">
         <v>36602</v>
@@ -1249,7 +1284,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B68" s="2">
         <v>36610</v>
@@ -1260,7 +1295,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B69" s="2">
         <v>36616</v>
@@ -1271,7 +1306,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B70" s="2">
         <v>36630</v>
@@ -1282,7 +1317,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B71" s="2">
         <v>36658</v>
@@ -1293,7 +1328,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B72" s="2">
         <v>36669</v>
@@ -1304,7 +1339,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B73" s="2">
         <v>36546</v>
@@ -1315,7 +1350,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74" s="2">
         <v>36553</v>
@@ -1326,7 +1361,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B75" s="2">
         <v>36558</v>
@@ -1337,7 +1372,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B76" s="2">
         <v>36567</v>
@@ -1348,7 +1383,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B77" s="2">
         <v>36574</v>
@@ -1359,7 +1394,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B78" s="2">
         <v>36581</v>
@@ -1370,7 +1405,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B79" s="2">
         <v>36588</v>
@@ -1381,7 +1416,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B80" s="2">
         <v>36595</v>
@@ -1392,7 +1427,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B81" s="2">
         <v>36602</v>
@@ -1403,7 +1438,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B82" s="2">
         <v>36610</v>
@@ -1414,7 +1449,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B83" s="2">
         <v>36616</v>
@@ -1425,7 +1460,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B84" s="2">
         <v>36630</v>
@@ -1436,7 +1471,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B85" s="2">
         <v>36658</v>
@@ -1447,7 +1482,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B86" s="2">
         <v>36669</v>
@@ -1458,7 +1493,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B87" s="2">
         <v>36546</v>
@@ -1469,7 +1504,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B88" s="2">
         <v>36553</v>
@@ -1480,7 +1515,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B89" s="2">
         <v>36558</v>
@@ -1491,7 +1526,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B90" s="2">
         <v>36567</v>
@@ -1502,7 +1537,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B91" s="2">
         <v>36574</v>
@@ -1513,7 +1548,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B92" s="2">
         <v>36581</v>
@@ -1524,7 +1559,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B93" s="2">
         <v>36588</v>
@@ -1535,7 +1570,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B94" s="2">
         <v>36595</v>
@@ -1546,7 +1581,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B95" s="2">
         <v>36602</v>
@@ -1557,7 +1592,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B96" s="2">
         <v>36610</v>
@@ -1568,7 +1603,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B97" s="2">
         <v>36616</v>
@@ -1579,7 +1614,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B98" s="2">
         <v>36630</v>
@@ -1590,7 +1625,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B99" s="2">
         <v>36668</v>
@@ -1601,7 +1636,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B100" s="2">
         <v>36669</v>
@@ -1612,7 +1647,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B101" s="2">
         <v>36546</v>
@@ -1623,7 +1658,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B102" s="2">
         <v>36553</v>
@@ -1634,7 +1669,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B103" s="2">
         <v>36558</v>
@@ -1645,7 +1680,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B104" s="2">
         <v>36567</v>
@@ -1656,7 +1691,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B105" s="2">
         <v>36574</v>
@@ -1667,7 +1702,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B106" s="2">
         <v>36581</v>
@@ -1678,7 +1713,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B107" s="2">
         <v>36588</v>
@@ -1689,7 +1724,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B108" s="2">
         <v>36595</v>
@@ -1700,7 +1735,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B109" s="2">
         <v>36602</v>
@@ -1711,7 +1746,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B110" s="2">
         <v>36610</v>
@@ -1722,7 +1757,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B111" s="2">
         <v>36616</v>
@@ -1733,7 +1768,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B112" s="2">
         <v>36630</v>
@@ -1744,7 +1779,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B113" s="2">
         <v>36638</v>
@@ -1755,7 +1790,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B114" s="2">
         <v>36674</v>
@@ -1766,7 +1801,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B115" s="2">
         <v>36681</v>
@@ -1777,7 +1812,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B116" s="2">
         <v>36688</v>
@@ -1788,7 +1823,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B117" s="2">
         <v>36695</v>
@@ -1799,7 +1834,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B118" s="2">
         <v>36702</v>
@@ -1810,7 +1845,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B119" s="2">
         <v>36546</v>
@@ -1821,7 +1856,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B120" s="2">
         <v>36553</v>
@@ -1832,7 +1867,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B121" s="2">
         <v>36558</v>
@@ -1843,7 +1878,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B122" s="2">
         <v>36567</v>
@@ -1854,7 +1889,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B123" s="2">
         <v>36574</v>
@@ -1865,7 +1900,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B124" s="2">
         <v>36581</v>
@@ -1876,7 +1911,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B125" s="2">
         <v>36588</v>
@@ -1887,7 +1922,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B126" s="2">
         <v>36595</v>
@@ -1898,7 +1933,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B127" s="2">
         <v>36602</v>
@@ -1909,7 +1944,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B128" s="2">
         <v>36610</v>
@@ -1920,7 +1955,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B129" s="2">
         <v>36616</v>
@@ -1931,7 +1966,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B130" s="2">
         <v>36630</v>
@@ -1942,7 +1977,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B131" s="2">
         <v>36658</v>
@@ -1953,7 +1988,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B132" s="2">
         <v>36546</v>
@@ -1964,7 +1999,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B133" s="2">
         <v>36553</v>
@@ -1975,7 +2010,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B134" s="2">
         <v>36558</v>
@@ -1986,7 +2021,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B135" s="2">
         <v>36567</v>
@@ -1997,7 +2032,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B136" s="2">
         <v>36574</v>
@@ -2008,7 +2043,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B137" s="2">
         <v>36581</v>
@@ -2019,7 +2054,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B138" s="2">
         <v>36588</v>
@@ -2030,7 +2065,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B139" s="2">
         <v>36595</v>
@@ -2041,7 +2076,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B140" s="2">
         <v>36602</v>
@@ -2052,7 +2087,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B141" s="2">
         <v>36610</v>
@@ -2063,7 +2098,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B142" s="2">
         <v>36616</v>
@@ -2074,7 +2109,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B143" s="2">
         <v>36630</v>
@@ -2085,7 +2120,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B144" s="2">
         <v>36658</v>
@@ -2096,7 +2131,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B145" s="2">
         <v>36668</v>
@@ -2107,7 +2142,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B146" s="2">
         <v>36669</v>
@@ -2118,7 +2153,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B147" s="2">
         <v>36641</v>
@@ -2129,7 +2164,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B148" s="2">
         <v>36648</v>
@@ -2140,7 +2175,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B149" s="2">
         <v>36653</v>
@@ -2151,7 +2186,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B150" s="2">
         <v>36659</v>
@@ -2162,7 +2197,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B151" s="2">
         <v>36666</v>
@@ -2173,7 +2208,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B152" s="2">
         <v>36709</v>
@@ -2184,7 +2219,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B153" s="2">
         <v>36641</v>
@@ -2195,7 +2230,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B154" s="2">
         <v>36648</v>
@@ -2206,7 +2241,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B155" s="2">
         <v>36653</v>
@@ -2217,7 +2252,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B156" s="2">
         <v>36709</v>
@@ -2228,7 +2263,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B157" s="2">
         <v>36641</v>
@@ -2239,7 +2274,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B158" s="2">
         <v>36648</v>
@@ -2250,7 +2285,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B159" s="2">
         <v>36653</v>
@@ -2261,7 +2296,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B160" s="2">
         <v>36659</v>
@@ -2272,7 +2307,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B161" s="2">
         <v>36666</v>
@@ -2283,7 +2318,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B162" s="2">
         <v>36709</v>
@@ -2294,7 +2329,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B163" s="2">
         <v>36641</v>
@@ -2305,7 +2340,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B164" s="2">
         <v>36648</v>
@@ -2316,7 +2351,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B165" s="2">
         <v>36653</v>
@@ -2327,7 +2362,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B166" s="2">
         <v>36659</v>
@@ -2338,7 +2373,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B167" s="2">
         <v>36666</v>
@@ -2349,7 +2384,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B168" s="2">
         <v>36714</v>
@@ -2360,7 +2395,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B169" s="2">
         <v>36641</v>
@@ -2371,7 +2406,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B170" s="2">
         <v>36648</v>
@@ -2382,7 +2417,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B171" s="2">
         <v>36653</v>
@@ -2393,7 +2428,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B172" s="2">
         <v>36673</v>
@@ -2404,7 +2439,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B173" s="2">
         <v>36641</v>
@@ -2415,7 +2450,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B174" s="2">
         <v>36648</v>
@@ -2426,7 +2461,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B175" s="2">
         <v>36653</v>
@@ -2437,7 +2472,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B176" s="2">
         <v>36659</v>
@@ -2448,7 +2483,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B177" s="2">
         <v>36666</v>
@@ -2459,7 +2494,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B178" s="2">
         <v>36709</v>
@@ -2470,7 +2505,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B179" s="2">
         <v>36533</v>
@@ -2481,7 +2516,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B180" s="2">
         <v>36540</v>
@@ -2492,7 +2527,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B181" s="2">
         <v>36547</v>
@@ -2503,7 +2538,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B182" s="2">
         <v>36554</v>
@@ -2514,7 +2549,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B183" s="2">
         <v>36561</v>
@@ -2525,7 +2560,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B184" s="2">
         <v>36568</v>
@@ -2536,7 +2571,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B185" s="2">
         <v>36575</v>
@@ -2547,7 +2582,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B186" s="2">
         <v>36582</v>
@@ -2558,7 +2593,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B187" s="2">
         <v>36589</v>
@@ -2569,7 +2604,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B188" s="2">
         <v>36597</v>
@@ -2580,7 +2615,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B189" s="2">
         <v>36634</v>
@@ -2591,7 +2626,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B190" s="2">
         <v>36639</v>
@@ -2602,7 +2637,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B191" s="2">
         <v>36701</v>
@@ -2613,7 +2648,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B192" s="2">
         <v>36533</v>
@@ -2624,7 +2659,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B193" s="2">
         <v>36540</v>
@@ -2635,7 +2670,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B194" s="2">
         <v>36547</v>
@@ -2646,7 +2681,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B195" s="2">
         <v>36554</v>
@@ -2657,7 +2692,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B196" s="2">
         <v>36561</v>
@@ -2668,7 +2703,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B197" s="2">
         <v>36582</v>
@@ -2679,7 +2714,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B198" s="2">
         <v>36533</v>
@@ -2690,7 +2725,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B199" s="2">
         <v>36540</v>
@@ -2701,7 +2736,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B200" s="2">
         <v>36547</v>
@@ -2712,7 +2747,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B201" s="2">
         <v>36554</v>
@@ -2723,7 +2758,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B202" s="2">
         <v>36561</v>
@@ -2734,7 +2769,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B203" s="2">
         <v>36568</v>
@@ -2745,7 +2780,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B204" s="2">
         <v>36582</v>
@@ -2756,7 +2791,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B205" s="2">
         <v>36597</v>
@@ -2767,7 +2802,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B206" s="2">
         <v>36624</v>
@@ -2778,7 +2813,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B207" s="2">
         <v>36652</v>
@@ -2789,7 +2824,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B208" s="2">
         <v>36701</v>
@@ -2800,7 +2835,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B209" s="2">
         <v>36702</v>
@@ -2811,7 +2846,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B210" s="2">
         <v>36533</v>
@@ -2822,7 +2857,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B211" s="2">
         <v>36540</v>
@@ -2833,7 +2868,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B212" s="2">
         <v>36547</v>
@@ -2844,7 +2879,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B213" s="2">
         <v>36554</v>
@@ -2855,7 +2890,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B214" s="2">
         <v>36561</v>
@@ -2866,7 +2901,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B215" s="2">
         <v>36568</v>
@@ -2877,7 +2912,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B216" s="2">
         <v>36582</v>
@@ -2888,7 +2923,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B217" s="2">
         <v>36597</v>
@@ -2899,7 +2934,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B218" s="2">
         <v>36624</v>
@@ -2910,7 +2945,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B219" s="2">
         <v>36701</v>
@@ -2921,7 +2956,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B220" s="2">
         <v>36707</v>
@@ -2932,7 +2967,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B221" s="2">
         <v>36533</v>
@@ -2943,7 +2978,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B222" s="2">
         <v>36540</v>
@@ -2954,7 +2989,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B223" s="2">
         <v>36547</v>
@@ -2965,7 +3000,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B224" s="2">
         <v>36554</v>
@@ -2976,7 +3011,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B225" s="2">
         <v>36561</v>
@@ -2987,7 +3022,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B226" s="2">
         <v>36533</v>
@@ -2998,7 +3033,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B227" s="2">
         <v>36540</v>
@@ -3009,7 +3044,7 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B228" s="2">
         <v>36547</v>
@@ -3020,7 +3055,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B229" s="2">
         <v>36554</v>
@@ -3031,7 +3066,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B230" s="2">
         <v>36561</v>
@@ -3042,7 +3077,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B231" s="2">
         <v>36568</v>
@@ -3053,7 +3088,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B232" s="2">
         <v>36575</v>
@@ -3064,7 +3099,7 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B233" s="2">
         <v>36582</v>
@@ -3075,7 +3110,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B234" s="2">
         <v>36597</v>
@@ -3086,7 +3121,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B235" s="2">
         <v>36634</v>
@@ -3097,7 +3132,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B236" s="2">
         <v>36638</v>
@@ -3108,7 +3143,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B237" s="2">
         <v>36639</v>
@@ -3119,10 +3154,10 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C238" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D238">
         <v>9.1363636363636367</v>
@@ -3136,10 +3171,10 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C239" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D239">
         <v>15.19047619047619</v>
@@ -3153,10 +3188,10 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C240" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D240">
         <v>14.27272727272727</v>
@@ -3170,10 +3205,10 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C241" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D241">
         <v>15.625</v>
@@ -3187,10 +3222,10 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C242" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D242">
         <v>6.6521739130434776</v>
@@ -3204,10 +3239,10 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C243" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D243">
         <v>6.935483870967742</v>
@@ -3221,10 +3256,10 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C244" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D244">
         <v>7.5454545454545459</v>
@@ -3238,10 +3273,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C245" t="s">
         <v>27</v>
-      </c>
-      <c r="C245" t="s">
-        <v>28</v>
       </c>
       <c r="D245">
         <v>10.71428571428571</v>
@@ -3255,10 +3290,10 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C246" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D246">
         <v>8.2777777777777786</v>
@@ -3272,10 +3307,10 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C247" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D247">
         <v>15.5</v>
@@ -3289,10 +3324,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C248" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D248">
         <v>7.9473684210526319</v>
@@ -3306,10 +3341,10 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C249" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D249">
         <v>8</v>
@@ -3323,10 +3358,10 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C250" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D250">
         <v>11.34285714285714</v>
@@ -3340,10 +3375,10 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C251" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D251">
         <v>16.358974358974361</v>
@@ -3357,10 +3392,10 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C252" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D252">
         <v>14.24444444444444</v>
@@ -3374,10 +3409,10 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C253" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D253">
         <v>16.844444444444441</v>
@@ -3391,10 +3426,10 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C254" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D254">
         <v>9.1111111111111107</v>
@@ -3408,10 +3443,10 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C255" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D255">
         <v>8.3552631578947363</v>
@@ -3425,10 +3460,10 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C256" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D256">
         <v>10.256410256410261</v>
@@ -3442,10 +3477,10 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C257" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D257">
         <v>11.133333333333329</v>
@@ -3459,10 +3494,10 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C258" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D258">
         <v>12.025</v>
@@ -3476,10 +3511,10 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C259" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D259">
         <v>13.5</v>
@@ -3493,10 +3528,10 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C260" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D260">
         <v>11.75</v>
@@ -3510,10 +3545,10 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C261" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D261">
         <v>12.141025641025641</v>

</xml_diff>

<commit_message>
Fixing header names and non numeric blank cells
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE8FC9-537E-4DFE-BD83-973DEF0F0569}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65A8BDF-74CF-4B75-9F94-1E7CE0328567}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,7 +3160,7 @@
         <v>27</v>
       </c>
       <c r="D238">
-        <v>9.1363636363636367</v>
+        <v>9.1363636360000005</v>
       </c>
       <c r="F238">
         <v>3.7057851239669422</v>
@@ -3177,7 +3177,7 @@
         <v>27</v>
       </c>
       <c r="D239">
-        <v>15.19047619047619</v>
+        <v>15.19047619</v>
       </c>
       <c r="F239">
         <v>9.2095238095238088</v>
@@ -3194,7 +3194,7 @@
         <v>27</v>
       </c>
       <c r="D240">
-        <v>14.27272727272727</v>
+        <v>14.272727270000001</v>
       </c>
       <c r="F240">
         <v>8.375206611570249</v>
@@ -3228,7 +3228,7 @@
         <v>27</v>
       </c>
       <c r="D242">
-        <v>6.6521739130434776</v>
+        <v>6.6521739130000004</v>
       </c>
       <c r="F242">
         <v>2.2292490118577071</v>
@@ -3245,7 +3245,7 @@
         <v>27</v>
       </c>
       <c r="D243">
-        <v>6.935483870967742</v>
+        <v>6.9354838709999997</v>
       </c>
       <c r="F243">
         <v>2.4868035190615831</v>
@@ -3262,7 +3262,7 @@
         <v>27</v>
       </c>
       <c r="D244">
-        <v>7.5454545454545459</v>
+        <v>7.5454545450000001</v>
       </c>
       <c r="F244">
         <v>3.041322314049586</v>
@@ -3279,7 +3279,7 @@
         <v>27</v>
       </c>
       <c r="D245">
-        <v>10.71428571428571</v>
+        <v>10.71428571</v>
       </c>
       <c r="F245">
         <v>5.9220779220779196</v>
@@ -3296,7 +3296,7 @@
         <v>27</v>
       </c>
       <c r="D246">
-        <v>8.2777777777777786</v>
+        <v>8.2777777780000008</v>
       </c>
       <c r="F246">
         <v>2.9252525252525259</v>
@@ -3330,7 +3330,7 @@
         <v>27</v>
       </c>
       <c r="D248">
-        <v>7.9473684210526319</v>
+        <v>7.9473684210000002</v>
       </c>
       <c r="F248">
         <v>2.6248803827751201</v>
@@ -3364,7 +3364,7 @@
         <v>27</v>
       </c>
       <c r="D250">
-        <v>11.34285714285714</v>
+        <v>11.34285714</v>
       </c>
       <c r="F250">
         <v>3.7025974025974029</v>
@@ -3381,7 +3381,7 @@
         <v>27</v>
       </c>
       <c r="D251">
-        <v>16.358974358974361</v>
+        <v>16.358974360000001</v>
       </c>
       <c r="F251">
         <v>8.2627039627039629</v>
@@ -3398,7 +3398,7 @@
         <v>27</v>
       </c>
       <c r="D252">
-        <v>14.24444444444444</v>
+        <v>14.244444440000001</v>
       </c>
       <c r="F252">
         <v>8.3767676767676758</v>
@@ -3415,7 +3415,7 @@
         <v>27</v>
       </c>
       <c r="D253">
-        <v>16.844444444444441</v>
+        <v>16.84444444</v>
       </c>
       <c r="F253">
         <v>10.740404040404041</v>
@@ -3432,7 +3432,7 @@
         <v>27</v>
       </c>
       <c r="D254">
-        <v>9.1111111111111107</v>
+        <v>9.1111111109999996</v>
       </c>
       <c r="F254">
         <v>2.2282828282828269</v>
@@ -3449,7 +3449,7 @@
         <v>27</v>
       </c>
       <c r="D255">
-        <v>8.3552631578947363</v>
+        <v>8.3552631579999996</v>
       </c>
       <c r="F255">
         <v>1.5411483253588509</v>
@@ -3466,7 +3466,7 @@
         <v>27</v>
       </c>
       <c r="D256">
-        <v>10.256410256410261</v>
+        <v>10.256410259999999</v>
       </c>
       <c r="F256">
         <v>3.0421911421911432</v>
@@ -3483,7 +3483,7 @@
         <v>27</v>
       </c>
       <c r="D257">
-        <v>11.133333333333329</v>
+        <v>11.133333329999999</v>
       </c>
       <c r="F257">
         <v>3.8393939393939398</v>
@@ -3551,7 +3551,7 @@
         <v>27</v>
       </c>
       <c r="D261">
-        <v>12.141025641025641</v>
+        <v>12.141025640000001</v>
       </c>
       <c r="F261">
         <v>2.9827505827505818</v>

</xml_diff>

<commit_message>
Add data for a few other cultivars in CE experiments
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A79305-9293-472E-99FA-AF9F8E0609E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16605" windowHeight="10530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="27825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="59">
   <si>
     <t>Clock.Today</t>
   </si>
@@ -115,16 +127,97 @@
   </si>
   <si>
     <t>Wheat.Phenology.FinalLeafNumber</t>
+  </si>
+  <si>
+    <t>Claire</t>
+  </si>
+  <si>
+    <t>Mccubbin</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLVCvClaireDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLNCvClaireDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSVCvClaireDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSNCvClaireDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLVCvMccubbinDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLNCvMccubbinDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSVCvMccubbinDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSNCvMccubbinDurat12</t>
+  </si>
+  <si>
+    <t>Amarok</t>
+  </si>
+  <si>
+    <t>Otane</t>
+  </si>
+  <si>
+    <t>Saracen</t>
+  </si>
+  <si>
+    <t>Rongotea</t>
+  </si>
+  <si>
+    <t>Wakanui</t>
+  </si>
+  <si>
+    <t>CRWT153</t>
+  </si>
+  <si>
+    <t>BattenWinter</t>
+  </si>
+  <si>
+    <t>BattenSpring</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLVCvRongoteaDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLNCvRongoteaDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSVCvRongoteaDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSNCvRongoteaDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLVCvWakanuiDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatLNCvWakanuiDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSVCvWakanuiDurat12</t>
+  </si>
+  <si>
+    <t>LincolnCETreatSNCvWakanuiDurat12</t>
+  </si>
+  <si>
+    <t>Wheat.SowingData.Cultivar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +233,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,16 +273,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,6 +393,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -310,6 +445,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -485,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G261"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
-      <selection activeCell="F268" sqref="F268"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +650,7 @@
     <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -520,8 +672,11 @@
       <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -532,7 +687,7 @@
         <v>2.5483333333333329</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -543,7 +698,7 @@
         <v>4.2844976282880554</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -554,7 +709,7 @@
         <v>5.0721482066892554</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -565,7 +720,7 @@
         <v>6.8495119318274291</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,7 +731,7 @@
         <v>7.5198160243152641</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -587,7 +742,7 @@
         <v>8.8199906302193956</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -598,7 +753,7 @@
         <v>9.4641138780746363</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -609,7 +764,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -620,7 +775,7 @@
         <v>12.33333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -631,7 +786,7 @@
         <v>2.027840351393797</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -642,7 +797,7 @@
         <v>3.3537310665417022</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -653,7 +808,7 @@
         <v>4.719348659003832</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -664,7 +819,7 @@
         <v>5.7779991587670372</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -675,7 +830,7 @@
         <v>6.591597796143251</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2974,7 +3129,7 @@
         <v>7.1024332234137759</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>26</v>
       </c>
@@ -2985,7 +3140,7 @@
         <v>6.9333333333333336</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>27</v>
       </c>
@@ -2996,7 +3151,7 @@
         <v>1.1384510869565221</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>27</v>
       </c>
@@ -3007,7 +3162,7 @@
         <v>2.803957718780727</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>27</v>
       </c>
@@ -3018,7 +3173,7 @@
         <v>4.5343486470189003</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>27</v>
       </c>
@@ -3029,7 +3184,7 @@
         <v>4.8236002068913333</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>27</v>
       </c>
@@ -3040,7 +3195,7 @@
         <v>5.6993572708522118</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>27</v>
       </c>
@@ -3051,7 +3206,7 @@
         <v>6.3563758708426272</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>27</v>
       </c>
@@ -3062,7 +3217,7 @@
         <v>7.0581054139054258</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>27</v>
       </c>
@@ -3073,7 +3228,7 @@
         <v>7.9261849403549496</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>27</v>
       </c>
@@ -3084,7 +3239,7 @@
         <v>8.6548773514044743</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>27</v>
       </c>
@@ -3095,7 +3250,7 @@
         <v>11.33333333333333</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>27</v>
       </c>
@@ -3106,7 +3261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>27</v>
       </c>
@@ -3117,7 +3272,7 @@
         <v>11.18181818181818</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>16</v>
       </c>
@@ -3133,8 +3288,11 @@
       <c r="G238">
         <v>5.7057851239669422</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H238" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>22</v>
       </c>
@@ -3150,8 +3308,11 @@
       <c r="G239">
         <v>11.209523809523811</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H239" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>19</v>
       </c>
@@ -3167,8 +3328,11 @@
       <c r="G240">
         <v>10.375206611570251</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H240" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>25</v>
       </c>
@@ -3184,8 +3348,11 @@
       <c r="G241">
         <v>11.60454545454545</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H241" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>20</v>
       </c>
@@ -3201,8 +3368,11 @@
       <c r="G242">
         <v>4.2292490118577071</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H242" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>26</v>
       </c>
@@ -3218,8 +3388,11 @@
       <c r="G243">
         <v>4.4868035190615831</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H243" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>21</v>
       </c>
@@ -3235,8 +3408,11 @@
       <c r="G244">
         <v>5.0413223140495864</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H244" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>27</v>
       </c>
@@ -3252,8 +3428,11 @@
       <c r="G245">
         <v>7.9220779220779196</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H245" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>18</v>
       </c>
@@ -3269,8 +3448,11 @@
       <c r="G246">
         <v>4.9252525252525263</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H246" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>24</v>
       </c>
@@ -3286,8 +3468,11 @@
       <c r="G247">
         <v>11.49090909090909</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H247" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>17</v>
       </c>
@@ -3303,8 +3488,11 @@
       <c r="G248">
         <v>4.6248803827751201</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H248" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>23</v>
       </c>
@@ -3320,8 +3508,11 @@
       <c r="G249">
         <v>4.6727272727272728</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H249" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>4</v>
       </c>
@@ -3337,8 +3528,11 @@
       <c r="G250">
         <v>7.7116883116883121</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H250" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>10</v>
       </c>
@@ -3354,8 +3548,11 @@
       <c r="G251">
         <v>12.271794871794871</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H251" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>7</v>
       </c>
@@ -3371,8 +3568,11 @@
       <c r="G252">
         <v>10.34949494949495</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H252" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>13</v>
       </c>
@@ -3388,8 +3588,11 @@
       <c r="G253">
         <v>12.71313131313131</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H253" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>8</v>
       </c>
@@ -3405,8 +3608,11 @@
       <c r="G254">
         <v>6.4646464646464636</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H254" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>14</v>
       </c>
@@ -3422,8 +3628,11 @@
       <c r="G255">
         <v>5.777511961722487</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H255" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>9</v>
       </c>
@@ -3439,8 +3648,11 @@
       <c r="G256">
         <v>7.5058275058275061</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H256" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>15</v>
       </c>
@@ -3456,8 +3668,11 @@
       <c r="G257">
         <v>8.3030303030303028</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H257" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>6</v>
       </c>
@@ -3473,8 +3688,11 @@
       <c r="G258">
         <v>8.331818181818182</v>
       </c>
-    </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H258" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>12</v>
       </c>
@@ -3490,8 +3708,11 @@
       <c r="G259">
         <v>9.672727272727272</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H259" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>5</v>
       </c>
@@ -3507,8 +3728,11 @@
       <c r="G260">
         <v>8.081818181818182</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H260" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>11</v>
       </c>
@@ -3523,6 +3747,233 @@
       </c>
       <c r="G261">
         <v>8.4372960372960364</v>
+      </c>
+      <c r="H261" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C262" t="s">
+        <v>28</v>
+      </c>
+      <c r="D262">
+        <v>9</v>
+      </c>
+      <c r="H262" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C263" t="s">
+        <v>28</v>
+      </c>
+      <c r="D263">
+        <v>16</v>
+      </c>
+      <c r="H263" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C264" t="s">
+        <v>28</v>
+      </c>
+      <c r="D264">
+        <v>12</v>
+      </c>
+      <c r="H264" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C265" t="s">
+        <v>28</v>
+      </c>
+      <c r="D265">
+        <v>13</v>
+      </c>
+      <c r="H265" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C266" t="s">
+        <v>28</v>
+      </c>
+      <c r="D266">
+        <v>8</v>
+      </c>
+      <c r="H266" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C267" t="s">
+        <v>28</v>
+      </c>
+      <c r="D267">
+        <v>8</v>
+      </c>
+      <c r="H267" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C268" t="s">
+        <v>28</v>
+      </c>
+      <c r="D268">
+        <v>16</v>
+      </c>
+      <c r="H268" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A269" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C269" t="s">
+        <v>28</v>
+      </c>
+      <c r="D269">
+        <v>13</v>
+      </c>
+      <c r="H269" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C270" t="s">
+        <v>28</v>
+      </c>
+      <c r="D270">
+        <v>8</v>
+      </c>
+      <c r="H270" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A271" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C271" t="s">
+        <v>28</v>
+      </c>
+      <c r="D271">
+        <v>7</v>
+      </c>
+      <c r="H271" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C272" t="s">
+        <v>28</v>
+      </c>
+      <c r="D272">
+        <v>9</v>
+      </c>
+      <c r="H272" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C273" t="s">
+        <v>28</v>
+      </c>
+      <c r="D273">
+        <v>11</v>
+      </c>
+      <c r="H273" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C274" t="s">
+        <v>28</v>
+      </c>
+      <c r="D274">
+        <v>9.5</v>
+      </c>
+      <c r="H274" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A275" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C275" t="s">
+        <v>28</v>
+      </c>
+      <c r="D275">
+        <v>15</v>
+      </c>
+      <c r="H275" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A276" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C276" t="s">
+        <v>28</v>
+      </c>
+      <c r="D276">
+        <v>11</v>
+      </c>
+      <c r="H276" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A277" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C277" t="s">
+        <v>28</v>
+      </c>
+      <c r="D277">
+        <v>17</v>
+      </c>
+      <c r="H277" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove superfluous data columns from observed data and fix non matching variable names
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/LincolnCE_Obs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A79305-9293-472E-99FA-AF9F8E0609E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30227844-BC25-4708-BB91-661646A8C85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="27825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="48">
   <si>
     <t>Clock.Today</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Wheat.Phenology.FinalLeafNumber</t>
   </si>
   <si>
-    <t>Claire</t>
-  </si>
-  <si>
-    <t>Mccubbin</t>
-  </si>
-  <si>
     <t>LincolnCETreatLVCvClaireDurat12</t>
   </si>
   <si>
@@ -159,30 +153,6 @@
     <t>LincolnCETreatSNCvMccubbinDurat12</t>
   </si>
   <si>
-    <t>Amarok</t>
-  </si>
-  <si>
-    <t>Otane</t>
-  </si>
-  <si>
-    <t>Saracen</t>
-  </si>
-  <si>
-    <t>Rongotea</t>
-  </si>
-  <si>
-    <t>Wakanui</t>
-  </si>
-  <si>
-    <t>CRWT153</t>
-  </si>
-  <si>
-    <t>BattenWinter</t>
-  </si>
-  <si>
-    <t>BattenSpring</t>
-  </si>
-  <si>
     <t>LincolnCETreatLVCvRongoteaDurat12</t>
   </si>
   <si>
@@ -205,9 +175,6 @@
   </si>
   <si>
     <t>LincolnCETreatSNCvWakanuiDurat12</t>
-  </si>
-  <si>
-    <t>Wheat.SowingData.Cultivar</t>
   </si>
 </sst>
 </file>
@@ -217,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,14 +199,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -288,17 +247,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,9 +274,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,9 +314,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,26 +349,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,26 +384,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -638,19 +560,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H277"/>
+  <dimension ref="A1:G277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -672,11 +595,8 @@
       <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -687,7 +607,7 @@
         <v>2.5483333333333329</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -698,7 +618,7 @@
         <v>4.2844976282880554</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -709,7 +629,7 @@
         <v>5.0721482066892554</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -720,7 +640,7 @@
         <v>6.8495119318274291</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -731,7 +651,7 @@
         <v>7.5198160243152641</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -742,7 +662,7 @@
         <v>8.8199906302193956</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -753,7 +673,7 @@
         <v>9.4641138780746363</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -764,7 +684,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -775,7 +695,7 @@
         <v>12.33333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -786,7 +706,7 @@
         <v>2.027840351393797</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -797,7 +717,7 @@
         <v>3.3537310665417022</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -808,7 +728,7 @@
         <v>4.719348659003832</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -819,7 +739,7 @@
         <v>5.7779991587670372</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -830,7 +750,7 @@
         <v>6.591597796143251</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -841,7 +761,7 @@
         <v>7.2856263120692466</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -852,7 +772,7 @@
         <v>8.1647382531395518</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -863,7 +783,7 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -874,7 +794,7 @@
         <v>11.55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -885,7 +805,7 @@
         <v>2.2509784735812128</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -896,7 +816,7 @@
         <v>3.5225379715825582</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -907,7 +827,7 @@
         <v>4.602474226804123</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -918,7 +838,7 @@
         <v>5.6620049147152356</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -929,7 +849,7 @@
         <v>6.3939296845562161</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -940,7 +860,7 @@
         <v>7.1685511061217149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -951,7 +871,7 @@
         <v>8.0161402228036422</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -962,7 +882,7 @@
         <v>12.025</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -973,7 +893,7 @@
         <v>3.1202481665800739</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -984,7 +904,7 @@
         <v>4.2804315393015129</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -995,7 +915,7 @@
         <v>5.3589295987031296</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -1006,7 +926,7 @@
         <v>5.970673860292429</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1017,7 +937,7 @@
         <v>7.3336387436315569</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +948,7 @@
         <v>7.9388891238886137</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1039,7 +959,7 @@
         <v>8.9252376100533048</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1050,7 +970,7 @@
         <v>9.4707228535353529</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1061,7 +981,7 @@
         <v>12.133333333333329</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +992,7 @@
         <v>13.66666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1003,7 @@
         <v>13.928571428571431</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1094,7 +1014,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -1105,7 +1025,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -1127,7 +1047,7 @@
         <v>2.1891244725738401</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -1138,7 +1058,7 @@
         <v>3.4292452830188682</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1149,7 +1069,7 @@
         <v>4.936791612694301</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1160,7 +1080,7 @@
         <v>6.2490561868686862</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -1171,7 +1091,7 @@
         <v>7.1761904761904756</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -1182,7 +1102,7 @@
         <v>8.4238095238095241</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
@@ -1193,7 +1113,7 @@
         <v>9.3333333333333339</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1135,7 @@
         <v>2.0529404472976851</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
@@ -1226,7 +1146,7 @@
         <v>3.5012755102040809</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1157,7 @@
         <v>4.5943396226415096</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
@@ -1248,7 +1168,7 @@
         <v>5.5343945892444726</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
@@ -1259,7 +1179,7 @@
         <v>6.7397257539991564</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1190,7 @@
         <v>6.9905676091814746</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>9</v>
       </c>
@@ -1281,7 +1201,7 @@
         <v>7.7341010206752152</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>9</v>
       </c>
@@ -1292,7 +1212,7 @@
         <v>10.35</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1223,7 @@
         <v>10.157894736842101</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -1314,7 +1234,7 @@
         <v>3.0886898924099881</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
@@ -1325,7 +1245,7 @@
         <v>4.3650200535495838</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -1336,7 +1256,7 @@
         <v>5.0232794009714512</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>10</v>
       </c>
@@ -1347,7 +1267,7 @@
         <v>5.8412778413902329</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +1278,7 @@
         <v>6.9659802931308699</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>10</v>
       </c>
@@ -1369,7 +1289,7 @@
         <v>7.9907540770943184</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -1380,7 +1300,7 @@
         <v>8.6330352900828107</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>10</v>
       </c>
@@ -1391,7 +1311,7 @@
         <v>9.8598767858844738</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
@@ -1402,7 +1322,7 @@
         <v>11.22839940757212</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1333,7 @@
         <v>12.51106860614494</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
@@ -1424,7 +1344,7 @@
         <v>12.72091443112301</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>10</v>
       </c>
@@ -1435,7 +1355,7 @@
         <v>12.94225443187784</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
@@ -1446,7 +1366,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
@@ -1457,7 +1377,7 @@
         <v>16.74074074074074</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>11</v>
       </c>
@@ -1468,7 +1388,7 @@
         <v>2.7819318786588609</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
@@ -1479,7 +1399,7 @@
         <v>3.6905626520355281</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1410,7 @@
         <v>4.3647824483497697</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -1501,7 +1421,7 @@
         <v>5.0826539527160746</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>11</v>
       </c>
@@ -1512,7 +1432,7 @@
         <v>6.238632385698204</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -1523,7 +1443,7 @@
         <v>6.8012716514225886</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1454,7 @@
         <v>7.6224941031658311</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>11</v>
       </c>
@@ -1545,7 +1465,7 @@
         <v>8.3991673812924681</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -1556,7 +1476,7 @@
         <v>8.9860870736655265</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1487,7 @@
         <v>10.089561310782241</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1498,7 @@
         <v>10.53762678632404</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -1589,7 +1509,7 @@
         <v>11.886516749852881</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
@@ -1600,7 +1520,7 @@
         <v>12.18333333333333</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>11</v>
       </c>
@@ -1611,7 +1531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -1622,7 +1542,7 @@
         <v>2.8606143598122769</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
@@ -1633,7 +1553,7 @@
         <v>3.9269604786520951</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
@@ -1644,7 +1564,7 @@
         <v>4.3036649082383374</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -1655,7 +1575,7 @@
         <v>5.3374275877575998</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1586,7 @@
         <v>6.229974485520966</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>12</v>
       </c>
@@ -1677,7 +1597,7 @@
         <v>6.918292467890037</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
@@ -1688,7 +1608,7 @@
         <v>7.5570938224465616</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>12</v>
       </c>
@@ -1699,7 +1619,7 @@
         <v>8.4349396445204832</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
@@ -1710,7 +1630,7 @@
         <v>8.7859021973632263</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1641,7 @@
         <v>10.14013495013843</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>12</v>
       </c>
@@ -1732,7 +1652,7 @@
         <v>10.34354844003215</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>12</v>
       </c>
@@ -1743,7 +1663,7 @@
         <v>12.353125</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
@@ -1754,7 +1674,7 @@
         <v>13.66666666666667</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>12</v>
       </c>
@@ -1765,7 +1685,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>13</v>
       </c>
@@ -1776,7 +1696,7 @@
         <v>3.0643755190266928</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>13</v>
       </c>
@@ -1787,7 +1707,7 @@
         <v>4.1263030138836436</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>13</v>
       </c>
@@ -1798,7 +1718,7 @@
         <v>4.8592823162016723</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>13</v>
       </c>
@@ -1809,7 +1729,7 @@
         <v>5.6369015120274311</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>13</v>
       </c>
@@ -1820,7 +1740,7 @@
         <v>6.8941529879598074</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>13</v>
       </c>
@@ -1831,7 +1751,7 @@
         <v>7.5390668915120864</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>13</v>
       </c>
@@ -1842,7 +1762,7 @@
         <v>8.6365677731240371</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>13</v>
       </c>
@@ -1853,7 +1773,7 @@
         <v>9.1801546678535662</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>13</v>
       </c>
@@ -1864,7 +1784,7 @@
         <v>10.75585572116479</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>13</v>
       </c>
@@ -1875,7 +1795,7 @@
         <v>11.489256592214261</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>13</v>
       </c>
@@ -1886,7 +1806,7 @@
         <v>12.21963457047641</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>13</v>
       </c>
@@ -1897,7 +1817,7 @@
         <v>13.600351690199631</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>13</v>
       </c>
@@ -1908,7 +1828,7 @@
         <v>13.414136115751081</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>13</v>
       </c>
@@ -1919,7 +1839,7 @@
         <v>15.89130434782609</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>13</v>
       </c>
@@ -1930,7 +1850,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>13</v>
       </c>
@@ -1941,7 +1861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>13</v>
       </c>
@@ -1952,7 +1872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>13</v>
       </c>
@@ -1963,7 +1883,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>14</v>
       </c>
@@ -1974,7 +1894,7 @@
         <v>3.5827241447717899</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>14</v>
       </c>
@@ -1985,7 +1905,7 @@
         <v>3.6390504322917798</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>14</v>
       </c>
@@ -1996,7 +1916,7 @@
         <v>4.8747897560850824</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>14</v>
       </c>
@@ -2007,7 +1927,7 @@
         <v>6.8308150183150174</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>14</v>
       </c>
@@ -2018,7 +1938,7 @@
         <v>8.5189280046771909</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>14</v>
       </c>
@@ -2029,7 +1949,7 @@
         <v>7.9285714285714288</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>14</v>
       </c>
@@ -2040,7 +1960,7 @@
         <v>8.125</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>14</v>
       </c>
@@ -2051,7 +1971,7 @@
         <v>8.4166666666666661</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>14</v>
       </c>
@@ -2062,7 +1982,7 @@
         <v>8.6666666666666661</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>14</v>
       </c>
@@ -2073,7 +1993,7 @@
         <v>8.3461538461538467</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>14</v>
       </c>
@@ -2084,7 +2004,7 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>14</v>
       </c>
@@ -2095,7 +2015,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>14</v>
       </c>
@@ -2106,7 +2026,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>15</v>
       </c>
@@ -2117,7 +2037,7 @@
         <v>2.8553111300054401</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>15</v>
       </c>
@@ -2128,7 +2048,7 @@
         <v>4.0086209188927446</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>15</v>
       </c>
@@ -2139,7 +2059,7 @@
         <v>4.6830639695027818</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>15</v>
       </c>
@@ -2150,7 +2070,7 @@
         <v>5.2896993216210024</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>15</v>
       </c>
@@ -2161,7 +2081,7 @@
         <v>6.4618935799721733</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>15</v>
       </c>
@@ -2172,7 +2092,7 @@
         <v>6.9404924435642767</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>15</v>
       </c>
@@ -2183,7 +2103,7 @@
         <v>7.644492906854274</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>15</v>
       </c>
@@ -2194,7 +2114,7 @@
         <v>8.4861137886775815</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>15</v>
       </c>
@@ -2205,7 +2125,7 @@
         <v>9.0155232076503999</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>15</v>
       </c>
@@ -2216,7 +2136,7 @@
         <v>10.37313875182323</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +2147,7 @@
         <v>10.191046767836641</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>15</v>
       </c>
@@ -2238,7 +2158,7 @@
         <v>11.236072463768121</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>15</v>
       </c>
@@ -2249,7 +2169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>15</v>
       </c>
@@ -2260,7 +2180,7 @@
         <v>11.21875</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>15</v>
       </c>
@@ -2271,7 +2191,7 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>16</v>
       </c>
@@ -2282,7 +2202,7 @@
         <v>3.2426545074349442</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>16</v>
       </c>
@@ -2293,7 +2213,7 @@
         <v>4.48626953737518</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>16</v>
       </c>
@@ -2304,7 +2224,7 @@
         <v>5.444625222368928</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>16</v>
       </c>
@@ -2315,7 +2235,7 @@
         <v>6.6971013655600196</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>16</v>
       </c>
@@ -2326,7 +2246,7 @@
         <v>8.2021306402922747</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>16</v>
       </c>
@@ -2337,7 +2257,7 @@
         <v>9.1578947368421044</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>17</v>
       </c>
@@ -2348,7 +2268,7 @@
         <v>2.7787500000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>17</v>
       </c>
@@ -2359,7 +2279,7 @@
         <v>4.3494437908496728</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>17</v>
       </c>
@@ -2370,7 +2290,7 @@
         <v>4.6023333333333341</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>17</v>
       </c>
@@ -2381,7 +2301,7 @@
         <v>7.9473684210526319</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>18</v>
       </c>
@@ -2392,7 +2312,7 @@
         <v>3.1404142638010462</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>18</v>
       </c>
@@ -2403,7 +2323,7 @@
         <v>4.7282645065767053</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>18</v>
       </c>
@@ -2414,7 +2334,7 @@
         <v>5.0451900284312172</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>18</v>
       </c>
@@ -2425,7 +2345,7 @@
         <v>6.4392975839150424</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>18</v>
       </c>
@@ -2436,7 +2356,7 @@
         <v>7.6193290063264527</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>18</v>
       </c>
@@ -2447,7 +2367,7 @@
         <v>8.3030303030303028</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>19</v>
       </c>
@@ -2458,7 +2378,7 @@
         <v>3.3239467068878832</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2389,7 @@
         <v>4.4022778071386259</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>19</v>
       </c>
@@ -2480,7 +2400,7 @@
         <v>5.2566661959981014</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>19</v>
       </c>
@@ -2491,7 +2411,7 @@
         <v>6.052695606280512</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>19</v>
       </c>
@@ -2502,7 +2422,7 @@
         <v>6.5659589794946651</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>19</v>
       </c>
@@ -2513,7 +2433,7 @@
         <v>14.27272727272727</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>20</v>
       </c>
@@ -2524,7 +2444,7 @@
         <v>2.915552044666688</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>20</v>
       </c>
@@ -2535,7 +2455,7 @@
         <v>4.7430105085677532</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>20</v>
       </c>
@@ -2546,7 +2466,7 @@
         <v>5.8327473631341036</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>20</v>
       </c>
@@ -2557,7 +2477,7 @@
         <v>6.6521739130434776</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>21</v>
       </c>
@@ -2568,7 +2488,7 @@
         <v>2.8152345224771178</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>21</v>
       </c>
@@ -2579,7 +2499,7 @@
         <v>4.322749860746435</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>21</v>
       </c>
@@ -2590,7 +2510,7 @@
         <v>5.0568347442250614</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>21</v>
       </c>
@@ -2601,7 +2521,7 @@
         <v>5.880703114774386</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>21</v>
       </c>
@@ -2612,7 +2532,7 @@
         <v>6.7460693604158868</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>21</v>
       </c>
@@ -2623,7 +2543,7 @@
         <v>7.65</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>22</v>
       </c>
@@ -2634,7 +2554,7 @@
         <v>2.0683142283648679</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>22</v>
       </c>
@@ -2645,7 +2565,7 @@
         <v>3.7387910691595572</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>22</v>
       </c>
@@ -2656,7 +2576,7 @@
         <v>4.8639117265253136</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>22</v>
       </c>
@@ -2667,7 +2587,7 @@
         <v>5.4597284151249843</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>22</v>
       </c>
@@ -2678,7 +2598,7 @@
         <v>6.5159281545179049</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>22</v>
       </c>
@@ -2689,7 +2609,7 @@
         <v>7.467388669728372</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>22</v>
       </c>
@@ -2700,7 +2620,7 @@
         <v>8.152922315109624</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>22</v>
       </c>
@@ -2711,7 +2631,7 @@
         <v>9.1478310254558952</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>22</v>
       </c>
@@ -2722,7 +2642,7 @@
         <v>10.11607252766578</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>22</v>
       </c>
@@ -2733,7 +2653,7 @@
         <v>10.44753380357443</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>22</v>
       </c>
@@ -2744,7 +2664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>22</v>
       </c>
@@ -2755,7 +2675,7 @@
         <v>15.33333333333333</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>22</v>
       </c>
@@ -2766,7 +2686,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>23</v>
       </c>
@@ -2777,7 +2697,7 @@
         <v>1.1816414828576769</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>23</v>
       </c>
@@ -2788,7 +2708,7 @@
         <v>2.707680336754799</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>23</v>
       </c>
@@ -2799,7 +2719,7 @@
         <v>3.9284457478005872</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>23</v>
       </c>
@@ -2810,7 +2730,7 @@
         <v>5.3121507369118266</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>23</v>
       </c>
@@ -2821,7 +2741,7 @@
         <v>7.1226175260060556</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>23</v>
       </c>
@@ -2832,7 +2752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>24</v>
       </c>
@@ -2843,7 +2763,7 @@
         <v>1.4722105913153081</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>24</v>
       </c>
@@ -2854,7 +2774,7 @@
         <v>2.737906131181342</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>24</v>
       </c>
@@ -2865,7 +2785,7 @@
         <v>4.815872964956653</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>24</v>
       </c>
@@ -2876,7 +2796,7 @@
         <v>4.8303766321983499</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>24</v>
       </c>
@@ -2887,7 +2807,7 @@
         <v>5.7757152849697126</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>24</v>
       </c>
@@ -2898,7 +2818,7 @@
         <v>6.6744291174652863</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>24</v>
       </c>
@@ -2909,7 +2829,7 @@
         <v>7.8747322636061252</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2840,7 @@
         <v>8.9069890151745561</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>24</v>
       </c>
@@ -2931,7 +2851,7 @@
         <v>13.022809917355371</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>24</v>
       </c>
@@ -2942,7 +2862,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>24</v>
       </c>
@@ -2953,7 +2873,7 @@
         <v>15.368421052631581</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>24</v>
       </c>
@@ -2964,7 +2884,7 @@
         <v>15.857142857142859</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>25</v>
       </c>
@@ -2975,7 +2895,7 @@
         <v>0.8541131159560752</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>25</v>
       </c>
@@ -2986,7 +2906,7 @@
         <v>2.6982924592028059</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>25</v>
       </c>
@@ -2997,7 +2917,7 @@
         <v>4.0628143638145016</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>25</v>
       </c>
@@ -3008,7 +2928,7 @@
         <v>5.4102377527709624</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>25</v>
       </c>
@@ -3019,7 +2939,7 @@
         <v>6.0263585278626159</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>25</v>
       </c>
@@ -3030,7 +2950,7 @@
         <v>6.8573075220291546</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>25</v>
       </c>
@@ -3041,7 +2961,7 @@
         <v>8.6402304926598852</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>25</v>
       </c>
@@ -3052,7 +2972,7 @@
         <v>9.765006244478025</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>25</v>
       </c>
@@ -3063,7 +2983,7 @@
         <v>13.20176767676768</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>25</v>
       </c>
@@ -3074,7 +2994,7 @@
         <v>15.52631578947368</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>25</v>
       </c>
@@ -3085,7 +3005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>26</v>
       </c>
@@ -3096,7 +3016,7 @@
         <v>1.4967387048782399</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>26</v>
       </c>
@@ -3107,7 +3027,7 @@
         <v>2.5869056847545222</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>26</v>
       </c>
@@ -3118,7 +3038,7 @@
         <v>6.314511986301369</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>26</v>
       </c>
@@ -3129,7 +3049,7 @@
         <v>7.1024332234137759</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>26</v>
       </c>
@@ -3140,7 +3060,7 @@
         <v>6.9333333333333336</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>27</v>
       </c>
@@ -3151,7 +3071,7 @@
         <v>1.1384510869565221</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>27</v>
       </c>
@@ -3162,7 +3082,7 @@
         <v>2.803957718780727</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>27</v>
       </c>
@@ -3173,7 +3093,7 @@
         <v>4.5343486470189003</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>27</v>
       </c>
@@ -3184,7 +3104,7 @@
         <v>4.8236002068913333</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>27</v>
       </c>
@@ -3195,7 +3115,7 @@
         <v>5.6993572708522118</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>27</v>
       </c>
@@ -3206,7 +3126,7 @@
         <v>6.3563758708426272</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>27</v>
       </c>
@@ -3217,7 +3137,7 @@
         <v>7.0581054139054258</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>27</v>
       </c>
@@ -3228,7 +3148,7 @@
         <v>7.9261849403549496</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>27</v>
       </c>
@@ -3239,7 +3159,7 @@
         <v>8.6548773514044743</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>27</v>
       </c>
@@ -3250,7 +3170,7 @@
         <v>11.33333333333333</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>27</v>
       </c>
@@ -3261,7 +3181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>27</v>
       </c>
@@ -3272,7 +3192,7 @@
         <v>11.18181818181818</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>16</v>
       </c>
@@ -3288,11 +3208,8 @@
       <c r="G238">
         <v>5.7057851239669422</v>
       </c>
-      <c r="H238" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>22</v>
       </c>
@@ -3308,11 +3225,8 @@
       <c r="G239">
         <v>11.209523809523811</v>
       </c>
-      <c r="H239" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>19</v>
       </c>
@@ -3328,11 +3242,8 @@
       <c r="G240">
         <v>10.375206611570251</v>
       </c>
-      <c r="H240" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>25</v>
       </c>
@@ -3348,11 +3259,8 @@
       <c r="G241">
         <v>11.60454545454545</v>
       </c>
-      <c r="H241" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>20</v>
       </c>
@@ -3368,11 +3276,8 @@
       <c r="G242">
         <v>4.2292490118577071</v>
       </c>
-      <c r="H242" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>26</v>
       </c>
@@ -3388,11 +3293,8 @@
       <c r="G243">
         <v>4.4868035190615831</v>
       </c>
-      <c r="H243" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>21</v>
       </c>
@@ -3408,11 +3310,8 @@
       <c r="G244">
         <v>5.0413223140495864</v>
       </c>
-      <c r="H244" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>27</v>
       </c>
@@ -3428,11 +3327,8 @@
       <c r="G245">
         <v>7.9220779220779196</v>
       </c>
-      <c r="H245" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>18</v>
       </c>
@@ -3448,11 +3344,8 @@
       <c r="G246">
         <v>4.9252525252525263</v>
       </c>
-      <c r="H246" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>24</v>
       </c>
@@ -3468,11 +3361,8 @@
       <c r="G247">
         <v>11.49090909090909</v>
       </c>
-      <c r="H247" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>17</v>
       </c>
@@ -3488,11 +3378,8 @@
       <c r="G248">
         <v>4.6248803827751201</v>
       </c>
-      <c r="H248" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>23</v>
       </c>
@@ -3508,11 +3395,8 @@
       <c r="G249">
         <v>4.6727272727272728</v>
       </c>
-      <c r="H249" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>4</v>
       </c>
@@ -3528,11 +3412,8 @@
       <c r="G250">
         <v>7.7116883116883121</v>
       </c>
-      <c r="H250" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>10</v>
       </c>
@@ -3548,11 +3429,8 @@
       <c r="G251">
         <v>12.271794871794871</v>
       </c>
-      <c r="H251" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>7</v>
       </c>
@@ -3568,11 +3446,8 @@
       <c r="G252">
         <v>10.34949494949495</v>
       </c>
-      <c r="H252" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>13</v>
       </c>
@@ -3588,11 +3463,8 @@
       <c r="G253">
         <v>12.71313131313131</v>
       </c>
-      <c r="H253" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>8</v>
       </c>
@@ -3608,11 +3480,8 @@
       <c r="G254">
         <v>6.4646464646464636</v>
       </c>
-      <c r="H254" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>14</v>
       </c>
@@ -3628,11 +3497,8 @@
       <c r="G255">
         <v>5.777511961722487</v>
       </c>
-      <c r="H255" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>9</v>
       </c>
@@ -3648,11 +3514,8 @@
       <c r="G256">
         <v>7.5058275058275061</v>
       </c>
-      <c r="H256" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>15</v>
       </c>
@@ -3668,11 +3531,8 @@
       <c r="G257">
         <v>8.3030303030303028</v>
       </c>
-      <c r="H257" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>6</v>
       </c>
@@ -3688,11 +3548,8 @@
       <c r="G258">
         <v>8.331818181818182</v>
       </c>
-      <c r="H258" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>12</v>
       </c>
@@ -3708,11 +3565,8 @@
       <c r="G259">
         <v>9.672727272727272</v>
       </c>
-      <c r="H259" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>5</v>
       </c>
@@ -3728,11 +3582,8 @@
       <c r="G260">
         <v>8.081818181818182</v>
       </c>
-      <c r="H260" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>11</v>
       </c>
@@ -3748,13 +3599,10 @@
       <c r="G261">
         <v>8.4372960372960364</v>
       </c>
-      <c r="H261" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C262" t="s">
         <v>28</v>
@@ -3762,13 +3610,10 @@
       <c r="D262">
         <v>9</v>
       </c>
-      <c r="H262" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C263" t="s">
         <v>28</v>
@@ -3776,13 +3621,10 @@
       <c r="D263">
         <v>16</v>
       </c>
-      <c r="H263" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C264" t="s">
         <v>28</v>
@@ -3790,13 +3632,10 @@
       <c r="D264">
         <v>12</v>
       </c>
-      <c r="H264" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C265" t="s">
         <v>28</v>
@@ -3804,13 +3643,10 @@
       <c r="D265">
         <v>13</v>
       </c>
-      <c r="H265" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C266" t="s">
         <v>28</v>
@@ -3818,13 +3654,10 @@
       <c r="D266">
         <v>8</v>
       </c>
-      <c r="H266" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C267" t="s">
         <v>28</v>
@@ -3832,13 +3665,10 @@
       <c r="D267">
         <v>8</v>
       </c>
-      <c r="H267" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C268" t="s">
         <v>28</v>
@@ -3846,13 +3676,10 @@
       <c r="D268">
         <v>16</v>
       </c>
-      <c r="H268" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C269" t="s">
         <v>28</v>
@@ -3860,13 +3687,10 @@
       <c r="D269">
         <v>13</v>
       </c>
-      <c r="H269" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C270" t="s">
         <v>28</v>
@@ -3874,13 +3698,10 @@
       <c r="D270">
         <v>8</v>
       </c>
-      <c r="H270" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C271" t="s">
         <v>28</v>
@@ -3888,13 +3709,10 @@
       <c r="D271">
         <v>7</v>
       </c>
-      <c r="H271" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C272" t="s">
         <v>28</v>
@@ -3902,13 +3720,10 @@
       <c r="D272">
         <v>9</v>
       </c>
-      <c r="H272" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C273" t="s">
         <v>28</v>
@@ -3916,13 +3731,10 @@
       <c r="D273">
         <v>11</v>
       </c>
-      <c r="H273" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C274" t="s">
         <v>28</v>
@@ -3930,13 +3742,10 @@
       <c r="D274">
         <v>9.5</v>
       </c>
-      <c r="H274" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C275" t="s">
         <v>28</v>
@@ -3944,13 +3753,10 @@
       <c r="D275">
         <v>15</v>
       </c>
-      <c r="H275" t="s">
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A276" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A276" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C276" t="s">
         <v>28</v>
@@ -3958,22 +3764,16 @@
       <c r="D276">
         <v>11</v>
       </c>
-      <c r="H276" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C277" t="s">
         <v>28</v>
       </c>
       <c r="D277">
         <v>17</v>
-      </c>
-      <c r="H277" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>